<commit_message>
started filling in table 1
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2410" documentId="8_{CEE25B56-0F43-46A5-82E3-B4208A1B7A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FBB2C62-E20B-4AE6-A946-057A79B4159C}"/>
+  <xr:revisionPtr revIDLastSave="2413" documentId="8_{CEE25B56-0F43-46A5-82E3-B4208A1B7A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A9FCF5E-FCAC-4415-9E76-86DB9F7FF228}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="2408" yWindow="3877" windowWidth="16875" windowHeight="10523" activeTab="3" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
@@ -11730,10 +11730,10 @@
     <t>Took less medicine than prescribed*</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: All numbers displayed in table are survey-weighted percentages (standard error). Bold face denotes statistically significant </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> differences (p &lt; 0.05) between CRN and no CRN within each disease category, as determined by t-tests or Rao-Scott Chi-Square tests.</t>
+    <t xml:space="preserve">Note: All numbers displayed in table are survey-weighted percentages (standard error) unless otherwise indicated. Bold face denotes statistically </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> significant differences (p &lt; 0.05) between CRN and no CRN within each disease category, as determined by t-tests or Rao-Scott Chi-Square tests.</t>
   </si>
 </sst>
 </file>
@@ -11983,15 +11983,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -12000,9 +11991,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12010,9 +11998,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12037,6 +12022,21 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12418,41 +12418,41 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="11"/>
       <c r="G1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="11"/>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="60" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="43"/>
+      <c r="M1" s="60"/>
       <c r="P1" s="11"/>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="60" t="s">
         <v>508</v>
       </c>
-      <c r="R1" s="43"/>
+      <c r="R1" s="60"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="43" t="s">
+      <c r="V1" s="60" t="s">
         <v>649</v>
       </c>
-      <c r="W1" s="43"/>
+      <c r="W1" s="60"/>
       <c r="Z1" s="11"/>
-      <c r="AA1" s="43" t="s">
+      <c r="AA1" s="60" t="s">
         <v>650</v>
       </c>
-      <c r="AB1" s="43"/>
+      <c r="AB1" s="60"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="43" t="s">
+      <c r="AF1" s="60" t="s">
         <v>659</v>
       </c>
-      <c r="AG1" s="43"/>
+      <c r="AG1" s="60"/>
       <c r="AJ1" s="11"/>
       <c r="AK1" s="29" t="s">
         <v>1045</v>
@@ -22270,47 +22270,47 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
       <c r="G1" s="11"/>
       <c r="H1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="29"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="60" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="43"/>
+      <c r="O1" s="60"/>
       <c r="Q1" s="29"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="43" t="s">
+      <c r="T1" s="60" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="43"/>
+      <c r="U1" s="60"/>
       <c r="W1" s="29"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="43" t="s">
+      <c r="Z1" s="60" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="43"/>
+      <c r="AA1" s="60"/>
       <c r="AC1" s="29"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="43" t="s">
+      <c r="AF1" s="60" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="43"/>
+      <c r="AG1" s="60"/>
       <c r="AI1" s="29"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="43" t="s">
+      <c r="AL1" s="60" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="43"/>
+      <c r="AM1" s="60"/>
       <c r="AO1" s="29"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="29" t="s">
@@ -32976,13 +32976,13 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
         <v>507</v>
@@ -32991,38 +32991,38 @@
       <c r="J1" s="6"/>
       <c r="K1" s="12"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="60" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="43"/>
+      <c r="O1" s="60"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="12"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="43" t="s">
+      <c r="T1" s="60" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="43"/>
+      <c r="U1" s="60"/>
       <c r="V1" s="6"/>
       <c r="W1" s="12"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="43" t="s">
+      <c r="Z1" s="60" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="43"/>
+      <c r="AA1" s="60"/>
       <c r="AB1" s="6"/>
       <c r="AC1" s="12"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="43" t="s">
+      <c r="AF1" s="60" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="43"/>
+      <c r="AG1" s="60"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="12"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="43" t="s">
+      <c r="AL1" s="60" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="43"/>
+      <c r="AM1" s="60"/>
       <c r="AO1" s="12"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="12" t="s">
@@ -45511,8 +45511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7B31CA-98BF-453E-B5B4-4EB9FEC3C9BB}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection sqref="A1:G41"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="87" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -45522,478 +45522,478 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="53"/>
-      <c r="B1" s="54" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="61" t="s">
         <v>3662</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61" t="s">
         <v>3877</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="E1" s="61"/>
+      <c r="F1" s="61" t="s">
         <v>3885</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="51" t="s">
         <v>3842</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="51" t="s">
         <v>3843</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="51" t="s">
         <v>3842</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="51" t="s">
         <v>3843</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="51" t="s">
         <v>3842</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="51" t="s">
         <v>3843</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="52" t="s">
         <v>3870</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="50" t="s">
         <v>3844</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="54" t="s">
         <v>3863</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="54" t="s">
         <v>3845</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="54" t="s">
         <v>3846</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="54" t="s">
         <v>3847</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="54" t="s">
         <v>3848</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="54" t="s">
         <v>3849</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="54" t="s">
         <v>3850</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="54" t="s">
         <v>3851</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="54" t="s">
         <v>3852</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="54" t="s">
         <v>3854</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="54" t="s">
         <v>3853</v>
       </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="54" t="s">
         <v>3855</v>
       </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="54" t="s">
         <v>3856</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="54" t="s">
         <v>3857</v>
       </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="54" t="s">
         <v>3858</v>
       </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="54" t="s">
         <v>3859</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="54" t="s">
         <v>3860</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="54" t="s">
         <v>3861</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="54" t="s">
         <v>3862</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="54" t="s">
         <v>3866</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="54" t="s">
         <v>3867</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="55" t="s">
         <v>3868</v>
       </c>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="56" t="s">
         <v>3864</v>
       </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="57" t="s">
         <v>3865</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="57" t="s">
         <v>3886</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="57" t="s">
         <v>3887</v>
       </c>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="62" t="s">
+      <c r="A38" s="57" t="s">
         <v>3888</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="58" t="s">
         <v>3889</v>
       </c>
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="57" t="s">
         <v>3890</v>
       </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="62" t="s">
+      <c r="A41" s="57" t="s">
         <v>3869</v>
       </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="53"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -46010,7 +46010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -46020,7 +46020,7 @@
     <col min="2" max="2" width="10.265625" style="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.796875" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.53125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" style="47" customWidth="1"/>
+    <col min="5" max="5" width="13.1328125" style="44" customWidth="1"/>
     <col min="6" max="6" width="2.86328125" style="32" customWidth="1"/>
     <col min="7" max="7" width="10.265625" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.796875" style="32" bestFit="1" customWidth="1"/>
@@ -46030,60 +46030,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="62" t="s">
         <v>3873</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="50" t="s">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="62" t="s">
         <v>3872</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:10" ht="29.25" x14ac:dyDescent="0.4">
       <c r="B2" s="42" t="s">
         <v>3875</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="45" t="s">
         <v>3876</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="45" t="s">
         <v>3881</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="45" t="s">
         <v>3882</v>
       </c>
       <c r="F2" s="42"/>
       <c r="G2" s="42" t="s">
         <v>3875</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="45" t="s">
         <v>3876</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="45" t="s">
         <v>3881</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="45" t="s">
         <v>3882</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="46" t="s">
         <v>3874</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="32" t="s">
@@ -46091,31 +46091,31 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="44" t="s">
         <v>3880</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="44" t="s">
         <v>3871</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="46" t="s">
         <v>3878</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="32" t="s">
@@ -46123,23 +46123,23 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="44" t="s">
         <v>3880</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="48" t="s">
         <v>3871</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="32" t="s">
@@ -46178,11 +46178,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -46419,20 +46419,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64" t="s">
         <v>3681</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B2" s="32" t="s">
@@ -46617,34 +46617,34 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="64"/>
+      <c r="C13" s="64" t="s">
         <v>3681</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="N13" s="45" t="s">
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="N13" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45" t="s">
+      <c r="O13" s="64"/>
+      <c r="P13" s="64" t="s">
         <v>3681</v>
       </c>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45" t="s">
+      <c r="Q13" s="64"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
+      <c r="T13" s="64"/>
+      <c r="U13" s="64"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B14" s="32" t="s">
@@ -47000,20 +47000,20 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45" t="s">
+      <c r="B25" s="64"/>
+      <c r="C25" s="64" t="s">
         <v>3681</v>
       </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45" t="s">
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B26" s="32" t="s">
@@ -47025,20 +47025,20 @@
       <c r="G26" s="32" t="s">
         <v>3699</v>
       </c>
-      <c r="N26" s="45" t="s">
+      <c r="N26" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45" t="s">
+      <c r="O26" s="64"/>
+      <c r="P26" s="64" t="s">
         <v>3681</v>
       </c>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45" t="s">
+      <c r="Q26" s="64"/>
+      <c r="R26" s="64"/>
+      <c r="S26" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
+      <c r="T26" s="64"/>
+      <c r="U26" s="64"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27" s="32" t="s">
@@ -47390,20 +47390,20 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="64" t="s">
         <v>3681</v>
       </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45" t="s">
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64" t="s">
         <v>377</v>
       </c>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B38" s="32" t="s">
@@ -47594,10 +47594,10 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="64" t="s">
         <v>3662</v>
       </c>
-      <c r="B48" s="45"/>
+      <c r="B48" s="64"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B49" s="32" t="s">
@@ -47692,18 +47692,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="C37:E37"/>
@@ -47711,6 +47699,18 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="F25:H25"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="S26:U26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -47718,21 +47718,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000918DFE69D23CA498FE8574F69332F5A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c85c3d5046845ec940253ce92485889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1ec804960e8faf3526f8b911669b534" ns3:_="">
     <xsd:import namespace="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
@@ -47878,10 +47863,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -47903,19 +47913,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed bmi and age to nonnormal
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2585" documentId="8_{CEE25B56-0F43-46A5-82E3-B4208A1B7A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{959B8193-F442-461C-9AD5-DFAA453CB2D5}"/>
+  <xr:revisionPtr revIDLastSave="2618" documentId="8_{CEE25B56-0F43-46A5-82E3-B4208A1B7A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F9E6127F-5532-4A6D-8652-9D757DFA4B50}"/>
   <bookViews>
-    <workbookView xWindow="2408" yWindow="3877" windowWidth="16875" windowHeight="10523" activeTab="3" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="6998" yWindow="5078" windowWidth="16875" windowHeight="10522" activeTab="3" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8395" uniqueCount="4101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8395" uniqueCount="4102">
   <si>
     <t>Variable</t>
   </si>
@@ -11832,24 +11832,12 @@
     <t>Medicare</t>
   </si>
   <si>
-    <t>63.75 (13.68)</t>
-  </si>
-  <si>
-    <t>54.58 (13.26)</t>
-  </si>
-  <si>
     <t>1071740.3 (52.2)</t>
   </si>
   <si>
     <t>779793.6 (61.2)</t>
   </si>
   <si>
-    <t>30.39 (5.72)</t>
-  </si>
-  <si>
-    <t>31.62 (6.17)</t>
-  </si>
-  <si>
     <t>362749.5 (17.7)</t>
   </si>
   <si>
@@ -11955,24 +11943,12 @@
     <t>248419.7 (12.1)</t>
   </si>
   <si>
-    <t>65.69 (15.53)</t>
-  </si>
-  <si>
-    <t>54.60 (15.04)</t>
-  </si>
-  <si>
     <t>1535387.7 (50.7)</t>
   </si>
   <si>
     <t>1178873.2 (62.2)</t>
   </si>
   <si>
-    <t>28.13 (5.42)</t>
-  </si>
-  <si>
-    <t>29.02 (6.13)</t>
-  </si>
-  <si>
     <t>546129.7 (18.0)</t>
   </si>
   <si>
@@ -12072,24 +12048,12 @@
     <t>413940.1 (13.7)</t>
   </si>
   <si>
-    <t>61.97 (15.69)</t>
-  </si>
-  <si>
-    <t>52.02 (14.68)</t>
-  </si>
-  <si>
     <t>4260646.5 (53.5)</t>
   </si>
   <si>
     <t>2653920.1 (62.9)</t>
   </si>
   <si>
-    <t>28.71 (5.45)</t>
-  </si>
-  <si>
-    <t>29.66 (6.11)</t>
-  </si>
-  <si>
     <t>1421081.4 (17.8)</t>
   </si>
   <si>
@@ -12364,13 +12328,52 @@
   </si>
   <si>
     <t>101008.8 2.4)</t>
+  </si>
+  <si>
+    <t>Age Median (IQR)</t>
+  </si>
+  <si>
+    <t>BMI Median (IQR)</t>
+  </si>
+  <si>
+    <t>65.00 [18.00, 85.00]</t>
+  </si>
+  <si>
+    <t>55.00 [18.00, 85.00]</t>
+  </si>
+  <si>
+    <t>29.80 [16.10, 53.90]</t>
+  </si>
+  <si>
+    <t>31.10 [17.30, 54.50]</t>
+  </si>
+  <si>
+    <t>68.00 [18.00, 85.00]</t>
+  </si>
+  <si>
+    <t>27.40 [14.80, 55.30]</t>
+  </si>
+  <si>
+    <t>28.20 [15.70, 54.50]</t>
+  </si>
+  <si>
+    <t>53.00 [18.00, 85.00]</t>
+  </si>
+  <si>
+    <t>64.00 [18.00, 85.00]</t>
+  </si>
+  <si>
+    <t>28.10 [14.80, 55.30]</t>
+  </si>
+  <si>
+    <t>29.00 [15.70, 54.50]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12453,14 +12456,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -12665,22 +12660,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12702,12 +12681,28 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13089,41 +13084,41 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
       <c r="F1" s="11"/>
       <c r="G1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="11"/>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="67" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="58"/>
+      <c r="M1" s="67"/>
       <c r="P1" s="11"/>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="67" t="s">
         <v>508</v>
       </c>
-      <c r="R1" s="58"/>
+      <c r="R1" s="67"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="58" t="s">
+      <c r="V1" s="67" t="s">
         <v>649</v>
       </c>
-      <c r="W1" s="58"/>
+      <c r="W1" s="67"/>
       <c r="Z1" s="11"/>
-      <c r="AA1" s="58" t="s">
+      <c r="AA1" s="67" t="s">
         <v>650</v>
       </c>
-      <c r="AB1" s="58"/>
+      <c r="AB1" s="67"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="58" t="s">
+      <c r="AF1" s="67" t="s">
         <v>659</v>
       </c>
-      <c r="AG1" s="58"/>
+      <c r="AG1" s="67"/>
       <c r="AJ1" s="11"/>
       <c r="AK1" s="29" t="s">
         <v>1045</v>
@@ -22941,47 +22936,47 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
       <c r="G1" s="11"/>
       <c r="H1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="29"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="58" t="s">
+      <c r="N1" s="67" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="58"/>
+      <c r="O1" s="67"/>
       <c r="Q1" s="29"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="67" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="58"/>
+      <c r="U1" s="67"/>
       <c r="W1" s="29"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="58" t="s">
+      <c r="Z1" s="67" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="58"/>
+      <c r="AA1" s="67"/>
       <c r="AC1" s="29"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="58" t="s">
+      <c r="AF1" s="67" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="58"/>
+      <c r="AG1" s="67"/>
       <c r="AI1" s="29"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="58" t="s">
+      <c r="AL1" s="67" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="58"/>
+      <c r="AM1" s="67"/>
       <c r="AO1" s="29"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="29" t="s">
@@ -33647,13 +33642,13 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
         <v>507</v>
@@ -33662,38 +33657,38 @@
       <c r="J1" s="6"/>
       <c r="K1" s="12"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="58" t="s">
+      <c r="N1" s="67" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="58"/>
+      <c r="O1" s="67"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="12"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="58" t="s">
+      <c r="T1" s="67" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="58"/>
+      <c r="U1" s="67"/>
       <c r="V1" s="6"/>
       <c r="W1" s="12"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="58" t="s">
+      <c r="Z1" s="67" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="58"/>
+      <c r="AA1" s="67"/>
       <c r="AB1" s="6"/>
       <c r="AC1" s="12"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="58" t="s">
+      <c r="AF1" s="67" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="58"/>
+      <c r="AG1" s="67"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="12"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="58" t="s">
+      <c r="AL1" s="67" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="58"/>
+      <c r="AM1" s="67"/>
       <c r="AO1" s="12"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="12" t="s">
@@ -46182,35 +46177,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7B31CA-98BF-453E-B5B4-4EB9FEC3C9BB}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="87" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.1328125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="12.53125" style="57" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.796875" style="57" customWidth="1"/>
-    <col min="4" max="4" width="12" style="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="57" customWidth="1"/>
-    <col min="6" max="6" width="12" style="57" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.86328125" style="57" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="57" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" style="57" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="57" customWidth="1"/>
+    <col min="5" max="5" width="14.73046875" style="57" customWidth="1"/>
+    <col min="6" max="6" width="14.1328125" style="57" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="57" customWidth="1"/>
     <col min="8" max="16384" width="9.06640625" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="68" t="s">
         <v>3662</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68" t="s">
         <v>3875</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59" t="s">
+      <c r="E1" s="68"/>
+      <c r="F1" s="68" t="s">
         <v>3883</v>
       </c>
-      <c r="G1" s="59"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="57" t="s">
@@ -46222,7 +46217,7 @@
       <c r="D2" s="57" t="s">
         <v>3842</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="58" t="s">
         <v>3843</v>
       </c>
       <c r="F2" s="57" t="s">
@@ -46236,830 +46231,830 @@
       <c r="A3" s="50" t="s">
         <v>3888</v>
       </c>
-      <c r="B3" s="66" t="s">
-        <v>4047</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>4048</v>
-      </c>
-      <c r="D3" s="66" t="s">
-        <v>4049</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>4050</v>
-      </c>
-      <c r="F3" s="66" t="s">
-        <v>4051</v>
-      </c>
-      <c r="G3" s="68" t="s">
-        <v>4052</v>
+      <c r="B3" s="60" t="s">
+        <v>4035</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>4036</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>4037</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>4038</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>4039</v>
+      </c>
+      <c r="G3" s="62" t="s">
+        <v>4040</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="69" t="s">
-        <v>3924</v>
-      </c>
-      <c r="C4" s="69" t="s">
-        <v>3923</v>
-      </c>
-      <c r="D4" s="69" t="s">
-        <v>3965</v>
-      </c>
-      <c r="E4" s="69" t="s">
-        <v>3964</v>
-      </c>
-      <c r="F4" s="69" t="s">
-        <v>4004</v>
-      </c>
-      <c r="G4" s="69" t="s">
-        <v>4003</v>
-      </c>
-      <c r="I4" s="65"/>
+        <v>4089</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>4092</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>4091</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>4092</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>4095</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>4098</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>4099</v>
+      </c>
+      <c r="I4" s="59"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="69" t="s">
-        <v>3926</v>
-      </c>
-      <c r="C5" s="69" t="s">
-        <v>3925</v>
-      </c>
-      <c r="D5" s="69" t="s">
-        <v>3967</v>
-      </c>
-      <c r="E5" s="69" t="s">
-        <v>3966</v>
-      </c>
-      <c r="F5" s="69" t="s">
-        <v>4006</v>
-      </c>
-      <c r="G5" s="69" t="s">
-        <v>4005</v>
-      </c>
-      <c r="I5" s="65"/>
+      <c r="B5" s="63" t="s">
+        <v>3924</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>3923</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>3961</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>3960</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>3996</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>3995</v>
+      </c>
+      <c r="I5" s="59"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>3928</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>3927</v>
-      </c>
-      <c r="D6" s="69" t="s">
-        <v>3969</v>
-      </c>
-      <c r="E6" s="69" t="s">
-        <v>3968</v>
-      </c>
-      <c r="F6" s="69" t="s">
-        <v>4008</v>
-      </c>
-      <c r="G6" s="69" t="s">
-        <v>4007</v>
-      </c>
-      <c r="I6" s="65"/>
+        <v>4090</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>4094</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>4093</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>4097</v>
+      </c>
+      <c r="E6" s="65" t="s">
+        <v>4096</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>4101</v>
+      </c>
+      <c r="G6" s="65" t="s">
+        <v>4100</v>
+      </c>
+      <c r="I6" s="59"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="I7" s="65"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="52" t="s">
         <v>3862</v>
       </c>
-      <c r="B8" s="69" t="s">
-        <v>3930</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>3929</v>
-      </c>
-      <c r="D8" s="69" t="s">
-        <v>3971</v>
-      </c>
-      <c r="E8" s="69" t="s">
-        <v>3970</v>
-      </c>
-      <c r="F8" s="69" t="s">
-        <v>4010</v>
-      </c>
-      <c r="G8" s="69" t="s">
-        <v>4009</v>
-      </c>
-      <c r="I8" s="65"/>
+      <c r="B8" s="63" t="s">
+        <v>3926</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>3925</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>3963</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>3962</v>
+      </c>
+      <c r="F8" s="63" t="s">
+        <v>3998</v>
+      </c>
+      <c r="G8" s="63" t="s">
+        <v>3997</v>
+      </c>
+      <c r="I8" s="59"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="52" t="s">
         <v>3844</v>
       </c>
-      <c r="B9" s="69" t="s">
-        <v>3932</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>3931</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>3973</v>
-      </c>
-      <c r="E9" s="69" t="s">
-        <v>3972</v>
-      </c>
-      <c r="F9" s="69" t="s">
-        <v>4012</v>
-      </c>
-      <c r="G9" s="69" t="s">
-        <v>4011</v>
-      </c>
-      <c r="I9" s="65"/>
+      <c r="B9" s="63" t="s">
+        <v>3928</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>3927</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>3965</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>3964</v>
+      </c>
+      <c r="F9" s="63" t="s">
+        <v>4000</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>3999</v>
+      </c>
+      <c r="I9" s="59"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="52" t="s">
         <v>3845</v>
       </c>
-      <c r="B10" s="69" t="s">
-        <v>3934</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>3933</v>
-      </c>
-      <c r="D10" s="69" t="s">
-        <v>3975</v>
-      </c>
-      <c r="E10" s="69" t="s">
-        <v>3974</v>
-      </c>
-      <c r="F10" s="69" t="s">
-        <v>4014</v>
-      </c>
-      <c r="G10" s="69" t="s">
-        <v>4013</v>
-      </c>
-      <c r="I10" s="65"/>
+      <c r="B10" s="63" t="s">
+        <v>3930</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>3929</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>3967</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>3966</v>
+      </c>
+      <c r="F10" s="63" t="s">
+        <v>4002</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>4001</v>
+      </c>
+      <c r="I10" s="59"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
         <v>3846</v>
       </c>
-      <c r="B11" s="69" t="s">
-        <v>3936</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>3935</v>
-      </c>
-      <c r="D11" s="69" t="s">
-        <v>3977</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>3976</v>
-      </c>
-      <c r="F11" s="69" t="s">
-        <v>4016</v>
-      </c>
-      <c r="G11" s="69" t="s">
-        <v>4015</v>
-      </c>
-      <c r="I11" s="65"/>
+      <c r="B11" s="63" t="s">
+        <v>3932</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>3931</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>3969</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>3968</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>4004</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>4003</v>
+      </c>
+      <c r="I11" s="59"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="I12" s="65"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="52" t="s">
         <v>3847</v>
       </c>
-      <c r="B13" s="69" t="s">
-        <v>3938</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>3937</v>
-      </c>
-      <c r="D13" s="69" t="s">
-        <v>3979</v>
-      </c>
-      <c r="E13" s="69" t="s">
-        <v>3978</v>
-      </c>
-      <c r="F13" s="69" t="s">
-        <v>4018</v>
-      </c>
-      <c r="G13" s="69" t="s">
-        <v>4017</v>
-      </c>
-      <c r="I13" s="65"/>
+      <c r="B13" s="63" t="s">
+        <v>3934</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>3933</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>3971</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>3970</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>4006</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>4005</v>
+      </c>
+      <c r="I13" s="59"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
         <v>3848</v>
       </c>
-      <c r="B14" s="69" t="s">
-        <v>3940</v>
-      </c>
-      <c r="C14" s="69" t="s">
-        <v>3939</v>
-      </c>
-      <c r="D14" s="69" t="s">
-        <v>3981</v>
-      </c>
-      <c r="E14" s="69" t="s">
-        <v>3980</v>
-      </c>
-      <c r="F14" s="69" t="s">
-        <v>4020</v>
-      </c>
-      <c r="G14" s="69" t="s">
-        <v>4019</v>
-      </c>
-      <c r="I14" s="65"/>
+      <c r="B14" s="63" t="s">
+        <v>3936</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>3935</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>3973</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>3972</v>
+      </c>
+      <c r="F14" s="63" t="s">
+        <v>4008</v>
+      </c>
+      <c r="G14" s="63" t="s">
+        <v>4007</v>
+      </c>
+      <c r="I14" s="59"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
         <v>3849</v>
       </c>
-      <c r="B15" s="69" t="s">
-        <v>3942</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>3941</v>
-      </c>
-      <c r="D15" s="69" t="s">
-        <v>4055</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>4056</v>
-      </c>
-      <c r="F15" s="69" t="s">
-        <v>4021</v>
-      </c>
-      <c r="G15" s="69" t="s">
-        <v>4057</v>
-      </c>
-      <c r="I15" s="65"/>
+      <c r="B15" s="63" t="s">
+        <v>3938</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>3937</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>4043</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>4044</v>
+      </c>
+      <c r="F15" s="63" t="s">
+        <v>4009</v>
+      </c>
+      <c r="G15" s="63" t="s">
+        <v>4045</v>
+      </c>
+      <c r="I15" s="59"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="52" t="s">
         <v>3850</v>
       </c>
-      <c r="B16" s="69" t="s">
-        <v>4058</v>
-      </c>
-      <c r="C16" s="69" t="s">
-        <v>4059</v>
-      </c>
-      <c r="D16" s="69" t="s">
-        <v>4060</v>
-      </c>
-      <c r="E16" s="69" t="s">
-        <v>4061</v>
-      </c>
-      <c r="F16" s="69" t="s">
-        <v>4062</v>
-      </c>
-      <c r="G16" s="69" t="s">
-        <v>4063</v>
-      </c>
-      <c r="I16" s="65"/>
+      <c r="B16" s="63" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>4047</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>4048</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>4049</v>
+      </c>
+      <c r="F16" s="63" t="s">
+        <v>4050</v>
+      </c>
+      <c r="G16" s="63" t="s">
+        <v>4051</v>
+      </c>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
         <v>3851</v>
       </c>
-      <c r="B17" s="69" t="s">
-        <v>4064</v>
-      </c>
-      <c r="C17" s="69" t="s">
-        <v>4065</v>
-      </c>
-      <c r="D17" s="69" t="s">
-        <v>4066</v>
-      </c>
-      <c r="E17" s="69" t="s">
-        <v>4067</v>
-      </c>
-      <c r="F17" s="69" t="s">
-        <v>4068</v>
-      </c>
-      <c r="G17" s="69" t="s">
-        <v>4069</v>
-      </c>
-      <c r="I17" s="65"/>
+      <c r="B17" s="63" t="s">
+        <v>4052</v>
+      </c>
+      <c r="C17" s="63" t="s">
+        <v>4053</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>4054</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>4055</v>
+      </c>
+      <c r="F17" s="63" t="s">
+        <v>4056</v>
+      </c>
+      <c r="G17" s="63" t="s">
+        <v>4057</v>
+      </c>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
         <v>3853</v>
       </c>
-      <c r="B18" s="69" t="s">
-        <v>4070</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>4071</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>4072</v>
-      </c>
-      <c r="E18" s="69" t="s">
-        <v>4073</v>
-      </c>
-      <c r="F18" s="69" t="s">
-        <v>4074</v>
-      </c>
-      <c r="G18" s="69" t="s">
-        <v>4075</v>
-      </c>
-      <c r="I18" s="65"/>
+      <c r="B18" s="63" t="s">
+        <v>4058</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>4060</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>4061</v>
+      </c>
+      <c r="F18" s="63" t="s">
+        <v>4062</v>
+      </c>
+      <c r="G18" s="63" t="s">
+        <v>4063</v>
+      </c>
+      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="I19" s="65"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="52" t="s">
         <v>3918</v>
       </c>
-      <c r="B20" s="69" t="s">
-        <v>3943</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>4053</v>
-      </c>
-      <c r="D20" s="69" t="s">
-        <v>3982</v>
-      </c>
-      <c r="E20" s="69" t="s">
-        <v>4076</v>
-      </c>
-      <c r="F20" s="69" t="s">
-        <v>4022</v>
-      </c>
-      <c r="G20" s="69" t="s">
-        <v>4077</v>
-      </c>
-      <c r="I20" s="65"/>
+      <c r="B20" s="63" t="s">
+        <v>3939</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>4041</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>3974</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>4064</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>4010</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>4065</v>
+      </c>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="52" t="s">
         <v>3919</v>
       </c>
-      <c r="B21" s="69" t="s">
-        <v>3945</v>
-      </c>
-      <c r="C21" s="69" t="s">
-        <v>3944</v>
-      </c>
-      <c r="D21" s="69" t="s">
-        <v>3984</v>
-      </c>
-      <c r="E21" s="69" t="s">
-        <v>3983</v>
-      </c>
-      <c r="F21" s="69" t="s">
-        <v>4024</v>
-      </c>
-      <c r="G21" s="69" t="s">
-        <v>4023</v>
-      </c>
-      <c r="I21" s="65"/>
+      <c r="B21" s="63" t="s">
+        <v>3941</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>3940</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>3976</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>3975</v>
+      </c>
+      <c r="F21" s="63" t="s">
+        <v>4012</v>
+      </c>
+      <c r="G21" s="63" t="s">
+        <v>4011</v>
+      </c>
+      <c r="I21" s="59"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="52" t="s">
         <v>3920</v>
       </c>
-      <c r="B22" s="69" t="s">
-        <v>3947</v>
-      </c>
-      <c r="C22" s="69" t="s">
-        <v>3946</v>
-      </c>
-      <c r="D22" s="69" t="s">
-        <v>3986</v>
-      </c>
-      <c r="E22" s="69" t="s">
-        <v>3985</v>
-      </c>
-      <c r="F22" s="69" t="s">
-        <v>4026</v>
-      </c>
-      <c r="G22" s="69" t="s">
-        <v>4025</v>
-      </c>
-      <c r="I22" s="65"/>
+      <c r="B22" s="63" t="s">
+        <v>3943</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>3942</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>3978</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>3977</v>
+      </c>
+      <c r="F22" s="63" t="s">
+        <v>4014</v>
+      </c>
+      <c r="G22" s="63" t="s">
+        <v>4013</v>
+      </c>
+      <c r="I22" s="59"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="52" t="s">
         <v>3921</v>
       </c>
-      <c r="B23" s="69" t="s">
-        <v>4078</v>
-      </c>
-      <c r="C23" s="69" t="s">
-        <v>4079</v>
-      </c>
-      <c r="D23" s="69" t="s">
-        <v>4080</v>
-      </c>
-      <c r="E23" s="69" t="s">
-        <v>4081</v>
-      </c>
-      <c r="F23" s="69" t="s">
-        <v>4082</v>
-      </c>
-      <c r="G23" s="69" t="s">
-        <v>4083</v>
-      </c>
-      <c r="I23" s="65"/>
+      <c r="B23" s="63" t="s">
+        <v>4066</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>4067</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>4068</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>4069</v>
+      </c>
+      <c r="F23" s="63" t="s">
+        <v>4070</v>
+      </c>
+      <c r="G23" s="63" t="s">
+        <v>4071</v>
+      </c>
+      <c r="I23" s="59"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="52" t="s">
         <v>3922</v>
       </c>
-      <c r="B24" s="69" t="s">
-        <v>3949</v>
-      </c>
-      <c r="C24" s="69" t="s">
-        <v>3948</v>
-      </c>
-      <c r="D24" s="69" t="s">
-        <v>3988</v>
-      </c>
-      <c r="E24" s="69" t="s">
-        <v>3987</v>
-      </c>
-      <c r="F24" s="69" t="s">
-        <v>4028</v>
-      </c>
-      <c r="G24" s="69" t="s">
-        <v>4027</v>
-      </c>
-      <c r="I24" s="65"/>
+      <c r="B24" s="63" t="s">
+        <v>3945</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>3944</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>3980</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>3979</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>4016</v>
+      </c>
+      <c r="G24" s="63" t="s">
+        <v>4015</v>
+      </c>
+      <c r="I24" s="59"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="52" t="s">
         <v>3853</v>
       </c>
-      <c r="B25" s="69" t="s">
-        <v>4084</v>
-      </c>
-      <c r="C25" s="69" t="s">
-        <v>4085</v>
-      </c>
-      <c r="D25" s="69" t="s">
-        <v>4086</v>
-      </c>
-      <c r="E25" s="69" t="s">
-        <v>4054</v>
-      </c>
-      <c r="F25" s="69" t="s">
-        <v>4087</v>
-      </c>
-      <c r="G25" s="69" t="s">
-        <v>4088</v>
-      </c>
-      <c r="I25" s="65"/>
+      <c r="B25" s="63" t="s">
+        <v>4072</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>4073</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>4074</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>4042</v>
+      </c>
+      <c r="F25" s="63" t="s">
+        <v>4075</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>4076</v>
+      </c>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="51" t="s">
         <v>194</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="I26" s="65"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="52" t="s">
         <v>3852</v>
       </c>
-      <c r="B27" s="69" t="s">
-        <v>3951</v>
-      </c>
-      <c r="C27" s="69" t="s">
-        <v>3950</v>
-      </c>
-      <c r="D27" s="69" t="s">
-        <v>3990</v>
-      </c>
-      <c r="E27" s="69" t="s">
-        <v>3989</v>
-      </c>
-      <c r="F27" s="69" t="s">
-        <v>4030</v>
-      </c>
-      <c r="G27" s="69" t="s">
-        <v>4029</v>
-      </c>
-      <c r="I27" s="65"/>
+      <c r="B27" s="63" t="s">
+        <v>3947</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>3946</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>3982</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>3981</v>
+      </c>
+      <c r="F27" s="63" t="s">
+        <v>4018</v>
+      </c>
+      <c r="G27" s="63" t="s">
+        <v>4017</v>
+      </c>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="52" t="s">
         <v>3854</v>
       </c>
-      <c r="B28" s="69" t="s">
-        <v>3953</v>
-      </c>
-      <c r="C28" s="69" t="s">
-        <v>3952</v>
-      </c>
-      <c r="D28" s="69" t="s">
-        <v>3992</v>
-      </c>
-      <c r="E28" s="69" t="s">
-        <v>3991</v>
-      </c>
-      <c r="F28" s="69" t="s">
-        <v>4032</v>
-      </c>
-      <c r="G28" s="69" t="s">
-        <v>4031</v>
-      </c>
-      <c r="I28" s="65"/>
+      <c r="B28" s="63" t="s">
+        <v>3949</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>3948</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>3984</v>
+      </c>
+      <c r="E28" s="63" t="s">
+        <v>3983</v>
+      </c>
+      <c r="F28" s="63" t="s">
+        <v>4020</v>
+      </c>
+      <c r="G28" s="63" t="s">
+        <v>4019</v>
+      </c>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="52" t="s">
         <v>3855</v>
       </c>
-      <c r="B29" s="69" t="s">
-        <v>3955</v>
-      </c>
-      <c r="C29" s="69" t="s">
-        <v>3954</v>
-      </c>
-      <c r="D29" s="69" t="s">
-        <v>3994</v>
-      </c>
-      <c r="E29" s="69" t="s">
-        <v>3993</v>
-      </c>
-      <c r="F29" s="69" t="s">
-        <v>4034</v>
-      </c>
-      <c r="G29" s="69" t="s">
-        <v>4033</v>
-      </c>
-      <c r="I29" s="65"/>
+      <c r="B29" s="63" t="s">
+        <v>3951</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>3950</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>3986</v>
+      </c>
+      <c r="E29" s="63" t="s">
+        <v>3985</v>
+      </c>
+      <c r="F29" s="63" t="s">
+        <v>4022</v>
+      </c>
+      <c r="G29" s="63" t="s">
+        <v>4021</v>
+      </c>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="I30" s="65"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="52" t="s">
         <v>3856</v>
       </c>
-      <c r="B31" s="69" t="s">
-        <v>3957</v>
-      </c>
-      <c r="C31" s="69" t="s">
-        <v>3956</v>
-      </c>
-      <c r="D31" s="69" t="s">
-        <v>3996</v>
-      </c>
-      <c r="E31" s="69" t="s">
-        <v>3995</v>
-      </c>
-      <c r="F31" s="69" t="s">
-        <v>4036</v>
-      </c>
-      <c r="G31" s="69" t="s">
-        <v>4035</v>
-      </c>
-      <c r="I31" s="65"/>
+      <c r="B31" s="63" t="s">
+        <v>3953</v>
+      </c>
+      <c r="C31" s="63" t="s">
+        <v>3952</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>3988</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>3987</v>
+      </c>
+      <c r="F31" s="63" t="s">
+        <v>4024</v>
+      </c>
+      <c r="G31" s="63" t="s">
+        <v>4023</v>
+      </c>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="52" t="s">
         <v>3857</v>
       </c>
-      <c r="B32" s="69" t="s">
-        <v>3959</v>
-      </c>
-      <c r="C32" s="69" t="s">
-        <v>3958</v>
-      </c>
-      <c r="D32" s="69" t="s">
-        <v>3998</v>
-      </c>
-      <c r="E32" s="69" t="s">
-        <v>3997</v>
-      </c>
-      <c r="F32" s="69" t="s">
-        <v>4038</v>
-      </c>
-      <c r="G32" s="69" t="s">
-        <v>4037</v>
-      </c>
-      <c r="I32" s="65"/>
+      <c r="B32" s="63" t="s">
+        <v>3955</v>
+      </c>
+      <c r="C32" s="63" t="s">
+        <v>3954</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>3990</v>
+      </c>
+      <c r="E32" s="63" t="s">
+        <v>3989</v>
+      </c>
+      <c r="F32" s="63" t="s">
+        <v>4026</v>
+      </c>
+      <c r="G32" s="63" t="s">
+        <v>4025</v>
+      </c>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="52" t="s">
         <v>3858</v>
       </c>
-      <c r="B33" s="69" t="s">
-        <v>3961</v>
-      </c>
-      <c r="C33" s="69" t="s">
-        <v>3960</v>
-      </c>
-      <c r="D33" s="69" t="s">
-        <v>4000</v>
-      </c>
-      <c r="E33" s="69" t="s">
-        <v>3999</v>
-      </c>
-      <c r="F33" s="69" t="s">
-        <v>4040</v>
-      </c>
-      <c r="G33" s="69" t="s">
-        <v>4039</v>
-      </c>
-      <c r="I33" s="65"/>
+      <c r="B33" s="63" t="s">
+        <v>3957</v>
+      </c>
+      <c r="C33" s="63" t="s">
+        <v>3956</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>3992</v>
+      </c>
+      <c r="E33" s="63" t="s">
+        <v>3991</v>
+      </c>
+      <c r="F33" s="63" t="s">
+        <v>4028</v>
+      </c>
+      <c r="G33" s="63" t="s">
+        <v>4027</v>
+      </c>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="52" t="s">
         <v>3859</v>
       </c>
-      <c r="B34" s="69" t="s">
-        <v>4089</v>
-      </c>
-      <c r="C34" s="69" t="s">
-        <v>3962</v>
-      </c>
-      <c r="D34" s="69" t="s">
-        <v>4090</v>
-      </c>
-      <c r="E34" s="69" t="s">
-        <v>4001</v>
-      </c>
-      <c r="F34" s="69" t="s">
-        <v>4091</v>
-      </c>
-      <c r="G34" s="69" t="s">
-        <v>4041</v>
-      </c>
-      <c r="I34" s="65"/>
+      <c r="B34" s="63" t="s">
+        <v>4077</v>
+      </c>
+      <c r="C34" s="63" t="s">
+        <v>3958</v>
+      </c>
+      <c r="D34" s="63" t="s">
+        <v>4078</v>
+      </c>
+      <c r="E34" s="63" t="s">
+        <v>3993</v>
+      </c>
+      <c r="F34" s="63" t="s">
+        <v>4079</v>
+      </c>
+      <c r="G34" s="63" t="s">
+        <v>4029</v>
+      </c>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="52" t="s">
         <v>3860</v>
       </c>
-      <c r="B35" s="69" t="s">
-        <v>4092</v>
-      </c>
-      <c r="C35" s="69" t="s">
-        <v>4093</v>
-      </c>
-      <c r="D35" s="69" t="s">
-        <v>4094</v>
-      </c>
-      <c r="E35" s="69" t="s">
-        <v>4095</v>
-      </c>
-      <c r="F35" s="69" t="s">
-        <v>4096</v>
-      </c>
-      <c r="G35" s="69" t="s">
-        <v>4097</v>
-      </c>
-      <c r="I35" s="65"/>
+      <c r="B35" s="63" t="s">
+        <v>4080</v>
+      </c>
+      <c r="C35" s="63" t="s">
+        <v>4081</v>
+      </c>
+      <c r="D35" s="63" t="s">
+        <v>4082</v>
+      </c>
+      <c r="E35" s="63" t="s">
+        <v>4083</v>
+      </c>
+      <c r="F35" s="63" t="s">
+        <v>4084</v>
+      </c>
+      <c r="G35" s="63" t="s">
+        <v>4085</v>
+      </c>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="52" t="s">
         <v>3861</v>
       </c>
-      <c r="B36" s="69" t="s">
-        <v>4098</v>
-      </c>
-      <c r="C36" s="69" t="s">
-        <v>3963</v>
-      </c>
-      <c r="D36" s="69" t="s">
-        <v>4099</v>
-      </c>
-      <c r="E36" s="69" t="s">
-        <v>4002</v>
-      </c>
-      <c r="F36" s="69" t="s">
-        <v>4100</v>
-      </c>
-      <c r="G36" s="69" t="s">
-        <v>4042</v>
-      </c>
-      <c r="I36" s="63"/>
+      <c r="B36" s="63" t="s">
+        <v>4086</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>3959</v>
+      </c>
+      <c r="D36" s="63" t="s">
+        <v>4087</v>
+      </c>
+      <c r="E36" s="63" t="s">
+        <v>3994</v>
+      </c>
+      <c r="F36" s="63" t="s">
+        <v>4088</v>
+      </c>
+      <c r="G36" s="63" t="s">
+        <v>4030</v>
+      </c>
+      <c r="I36" s="72"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="52" t="s">
         <v>3865</v>
       </c>
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="64" t="s">
         <v>3901</v>
       </c>
-      <c r="C38" s="70" t="s">
+      <c r="C38" s="64" t="s">
         <v>3900</v>
       </c>
-      <c r="D38" s="70" t="s">
+      <c r="D38" s="64" t="s">
         <v>3907</v>
       </c>
-      <c r="E38" s="71" t="s">
-        <v>4044</v>
-      </c>
-      <c r="F38" s="70" t="s">
+      <c r="E38" s="65" t="s">
+        <v>4032</v>
+      </c>
+      <c r="F38" s="64" t="s">
         <v>3917</v>
       </c>
-      <c r="G38" s="71" t="s">
-        <v>4045</v>
+      <c r="G38" s="65" t="s">
+        <v>4033</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="52" t="s">
         <v>3866</v>
       </c>
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="64" t="s">
         <v>3902</v>
       </c>
-      <c r="C39" s="70" t="s">
+      <c r="C39" s="64" t="s">
         <v>3903</v>
       </c>
-      <c r="D39" s="70" t="s">
+      <c r="D39" s="64" t="s">
         <v>3908</v>
       </c>
-      <c r="E39" s="71" t="s">
-        <v>4043</v>
-      </c>
-      <c r="F39" s="70" t="s">
+      <c r="E39" s="65" t="s">
+        <v>4031</v>
+      </c>
+      <c r="F39" s="64" t="s">
         <v>3916</v>
       </c>
-      <c r="G39" s="71" t="s">
-        <v>4046</v>
+      <c r="G39" s="65" t="s">
+        <v>4034</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="53" t="s">
         <v>3867</v>
       </c>
-      <c r="B40" s="70" t="s">
+      <c r="B40" s="64" t="s">
         <v>3904</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C40" s="64" t="s">
         <v>3905</v>
       </c>
-      <c r="D40" s="70" t="s">
+      <c r="D40" s="64" t="s">
         <v>3910</v>
       </c>
-      <c r="E40" s="72" t="s">
+      <c r="E40" s="66" t="s">
         <v>3909</v>
       </c>
-      <c r="F40" s="70" t="s">
+      <c r="F40" s="64" t="s">
         <v>3915</v>
       </c>
-      <c r="G40" s="72" t="s">
+      <c r="G40" s="66" t="s">
         <v>3914</v>
       </c>
     </row>
@@ -47072,22 +47067,22 @@
       <c r="A42" s="55" t="s">
         <v>3864</v>
       </c>
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="57" t="s">
         <v>3899</v>
       </c>
       <c r="C42" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="D42" s="70" t="s">
+      <c r="D42" s="57" t="s">
         <v>3906</v>
       </c>
-      <c r="E42" s="67" t="s">
+      <c r="E42" s="61" t="s">
         <v>3911</v>
       </c>
-      <c r="F42" s="70" t="s">
+      <c r="F42" s="57" t="s">
         <v>3913</v>
       </c>
-      <c r="G42" s="67" t="s">
+      <c r="G42" s="61" t="s">
         <v>3912</v>
       </c>
     </row>
@@ -47095,19 +47090,19 @@
       <c r="A43" s="55" t="s">
         <v>3884</v>
       </c>
-      <c r="B43" s="70" t="s">
+      <c r="B43" s="57" t="s">
         <v>3889</v>
       </c>
       <c r="C43" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="D43" s="70" t="s">
+      <c r="D43" s="57" t="s">
         <v>3893</v>
       </c>
       <c r="E43" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="F43" s="70" t="s">
+      <c r="F43" s="57" t="s">
         <v>3896</v>
       </c>
       <c r="G43" s="57" t="s">
@@ -47118,19 +47113,19 @@
       <c r="A44" s="55" t="s">
         <v>3885</v>
       </c>
-      <c r="B44" s="70" t="s">
+      <c r="B44" s="57" t="s">
         <v>3890</v>
       </c>
       <c r="C44" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="D44" s="70" t="s">
+      <c r="D44" s="57" t="s">
         <v>3894</v>
       </c>
       <c r="E44" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="F44" s="70" t="s">
+      <c r="F44" s="57" t="s">
         <v>3897</v>
       </c>
       <c r="G44" s="57" t="s">
@@ -47141,19 +47136,19 @@
       <c r="A45" s="55" t="s">
         <v>3886</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="57" t="s">
         <v>3891</v>
       </c>
       <c r="C45" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="D45" s="70" t="s">
+      <c r="D45" s="57" t="s">
         <v>3895</v>
       </c>
       <c r="E45" s="57" t="s">
         <v>3392</v>
       </c>
-      <c r="F45" s="70" t="s">
+      <c r="F45" s="57" t="s">
         <v>3898</v>
       </c>
       <c r="G45" s="57" t="s">
@@ -47164,12 +47159,12 @@
       <c r="A46" s="56" t="s">
         <v>3892</v>
       </c>
-      <c r="B46" s="66"/>
-      <c r="C46" s="66"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="66"/>
-      <c r="G46" s="66"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="55" t="s">
@@ -47216,19 +47211,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="69" t="s">
         <v>3871</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
       <c r="F1" s="47"/>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="69" t="s">
         <v>3870</v>
       </c>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
     </row>
     <row r="2" spans="1:10" ht="29.25" x14ac:dyDescent="0.4">
       <c r="B2" s="42" t="s">
@@ -47364,11 +47359,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -47605,20 +47600,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71" t="s">
         <v>3681</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62" t="s">
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B2" s="32" t="s">
@@ -47803,34 +47798,34 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62" t="s">
+      <c r="B13" s="71"/>
+      <c r="C13" s="71" t="s">
         <v>3681</v>
       </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62" t="s">
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="N13" s="62" t="s">
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="N13" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62" t="s">
+      <c r="O13" s="71"/>
+      <c r="P13" s="71" t="s">
         <v>3681</v>
       </c>
-      <c r="Q13" s="62"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="62" t="s">
+      <c r="Q13" s="71"/>
+      <c r="R13" s="71"/>
+      <c r="S13" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="T13" s="62"/>
-      <c r="U13" s="62"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="71"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B14" s="32" t="s">
@@ -48186,20 +48181,20 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62" t="s">
+      <c r="B25" s="71"/>
+      <c r="C25" s="71" t="s">
         <v>3681</v>
       </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62" t="s">
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B26" s="32" t="s">
@@ -48211,20 +48206,20 @@
       <c r="G26" s="32" t="s">
         <v>3699</v>
       </c>
-      <c r="N26" s="62" t="s">
+      <c r="N26" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="O26" s="62"/>
-      <c r="P26" s="62" t="s">
+      <c r="O26" s="71"/>
+      <c r="P26" s="71" t="s">
         <v>3681</v>
       </c>
-      <c r="Q26" s="62"/>
-      <c r="R26" s="62"/>
-      <c r="S26" s="62" t="s">
+      <c r="Q26" s="71"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="T26" s="62"/>
-      <c r="U26" s="62"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="71"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27" s="32" t="s">
@@ -48576,20 +48571,20 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62" t="s">
+      <c r="B37" s="71"/>
+      <c r="C37" s="71" t="s">
         <v>3681</v>
       </c>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62" t="s">
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B38" s="32" t="s">
@@ -48780,10 +48775,10 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A48" s="62" t="s">
+      <c r="A48" s="71" t="s">
         <v>3662</v>
       </c>
-      <c r="B48" s="62"/>
+      <c r="B48" s="71"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B49" s="32" t="s">
@@ -48878,6 +48873,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="C37:E37"/>
@@ -48885,18 +48892,6 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="F25:H25"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="S26:U26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -48904,6 +48899,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000918DFE69D23CA498FE8574F69332F5A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c85c3d5046845ec940253ce92485889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1ec804960e8faf3526f8b911669b534" ns3:_="">
     <xsd:import namespace="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
@@ -49049,35 +49059,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -49099,9 +49084,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ran the first round of models (for dz specific mortality)
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2618" documentId="8_{CEE25B56-0F43-46A5-82E3-B4208A1B7A72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F9E6127F-5532-4A6D-8652-9D757DFA4B50}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92D5B31-42A0-4DA4-AECA-20E419D46315}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6998" yWindow="5078" windowWidth="16875" windowHeight="10522" activeTab="3" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="7703" yWindow="1927" windowWidth="16875" windowHeight="10523" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8395" uniqueCount="4102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8407" uniqueCount="4114">
   <si>
     <t>Variable</t>
   </si>
@@ -11706,9 +11706,6 @@
     </r>
   </si>
   <si>
-    <t>1. Crude Hazard Ratio. 2. Adjusted for age, sex, race, insurance status, region, smoking status, and body mass index.</t>
-  </si>
-  <si>
     <t>Abbreviations: CRN, cost-related nonadherence; CVD, cardiovascular disease; IQR, interquartile range; HR, hazard ratio.</t>
   </si>
   <si>
@@ -12367,6 +12364,45 @@
   </si>
   <si>
     <t>29.00 [15.70, 54.50]</t>
+  </si>
+  <si>
+    <t>0.8018 (0.7004 - 0.9179)</t>
+  </si>
+  <si>
+    <t>0.7677 (0.6333 - 0.9307)</t>
+  </si>
+  <si>
+    <t>0.7792 (0.6393 - 0.9497)</t>
+  </si>
+  <si>
+    <t>1745 (3.11%)</t>
+  </si>
+  <si>
+    <t>804 (3.75%)</t>
+  </si>
+  <si>
+    <t>684 (4.31%)</t>
+  </si>
+  <si>
+    <t>1.2833 (1.0297 - 1.600)</t>
+  </si>
+  <si>
+    <t>1. Crude Hazard Ratio. 2. Adjusted for age, sex, insurance status, education, and income category.</t>
+  </si>
+  <si>
+    <t>1.5983 (1.29224 - 1.9769)</t>
+  </si>
+  <si>
+    <t>1.5593 (1.3499 - 1.8011)</t>
+  </si>
+  <si>
+    <t>308 (165 - 500)</t>
+  </si>
+  <si>
+    <t>326 (169 - 530)</t>
+  </si>
+  <si>
+    <t>348 (187 - 548)</t>
   </si>
 </sst>
 </file>
@@ -12687,6 +12723,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12702,7 +12739,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13084,41 +13120,41 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
       <c r="F1" s="11"/>
       <c r="G1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="11"/>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="68" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="67"/>
+      <c r="M1" s="68"/>
       <c r="P1" s="11"/>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="68" t="s">
         <v>508</v>
       </c>
-      <c r="R1" s="67"/>
+      <c r="R1" s="68"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="67" t="s">
+      <c r="V1" s="68" t="s">
         <v>649</v>
       </c>
-      <c r="W1" s="67"/>
+      <c r="W1" s="68"/>
       <c r="Z1" s="11"/>
-      <c r="AA1" s="67" t="s">
+      <c r="AA1" s="68" t="s">
         <v>650</v>
       </c>
-      <c r="AB1" s="67"/>
+      <c r="AB1" s="68"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="67" t="s">
+      <c r="AF1" s="68" t="s">
         <v>659</v>
       </c>
-      <c r="AG1" s="67"/>
+      <c r="AG1" s="68"/>
       <c r="AJ1" s="11"/>
       <c r="AK1" s="29" t="s">
         <v>1045</v>
@@ -22936,47 +22972,47 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
       <c r="G1" s="11"/>
       <c r="H1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="29"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="68" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="67"/>
+      <c r="O1" s="68"/>
       <c r="Q1" s="29"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="67" t="s">
+      <c r="T1" s="68" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="67"/>
+      <c r="U1" s="68"/>
       <c r="W1" s="29"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="67" t="s">
+      <c r="Z1" s="68" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="67"/>
+      <c r="AA1" s="68"/>
       <c r="AC1" s="29"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="67" t="s">
+      <c r="AF1" s="68" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="67"/>
+      <c r="AG1" s="68"/>
       <c r="AI1" s="29"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="67" t="s">
+      <c r="AL1" s="68" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="67"/>
+      <c r="AM1" s="68"/>
       <c r="AO1" s="29"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="29" t="s">
@@ -33642,13 +33678,13 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
         <v>507</v>
@@ -33657,38 +33693,38 @@
       <c r="J1" s="6"/>
       <c r="K1" s="12"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="68" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="67"/>
+      <c r="O1" s="68"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="12"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="67" t="s">
+      <c r="T1" s="68" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="67"/>
+      <c r="U1" s="68"/>
       <c r="V1" s="6"/>
       <c r="W1" s="12"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="67" t="s">
+      <c r="Z1" s="68" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="67"/>
+      <c r="AA1" s="68"/>
       <c r="AB1" s="6"/>
       <c r="AC1" s="12"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="67" t="s">
+      <c r="AF1" s="68" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="67"/>
+      <c r="AG1" s="68"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="12"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="67" t="s">
+      <c r="AL1" s="68" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="67"/>
+      <c r="AM1" s="68"/>
       <c r="AO1" s="12"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="12" t="s">
@@ -46177,8 +46213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7B31CA-98BF-453E-B5B4-4EB9FEC3C9BB}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.65" x14ac:dyDescent="0.35"/>
@@ -46194,18 +46230,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>3662</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="69" t="s">
         <v>3875</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68" t="s">
-        <v>3883</v>
-      </c>
-      <c r="G1" s="68"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69" t="s">
+        <v>3882</v>
+      </c>
+      <c r="G1" s="69"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="57" t="s">
@@ -46229,48 +46265,48 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="50" t="s">
-        <v>3888</v>
+        <v>3887</v>
       </c>
       <c r="B3" s="60" t="s">
+        <v>4034</v>
+      </c>
+      <c r="C3" s="60" t="s">
         <v>4035</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="D3" s="60" t="s">
         <v>4036</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="E3" s="61" t="s">
         <v>4037</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="F3" s="60" t="s">
         <v>4038</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="G3" s="62" t="s">
         <v>4039</v>
-      </c>
-      <c r="G3" s="62" t="s">
-        <v>4040</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="49" t="s">
-        <v>4089</v>
+        <v>4088</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>4092</v>
+        <v>4091</v>
       </c>
       <c r="C4" s="65" t="s">
+        <v>4090</v>
+      </c>
+      <c r="D4" s="65" t="s">
         <v>4091</v>
       </c>
-      <c r="D4" s="65" t="s">
-        <v>4092</v>
-      </c>
       <c r="E4" s="65" t="s">
-        <v>4095</v>
+        <v>4094</v>
       </c>
       <c r="F4" s="65" t="s">
+        <v>4097</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>4098</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>4099</v>
       </c>
       <c r="I4" s="59"/>
     </row>
@@ -46279,46 +46315,46 @@
         <v>128</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>3924</v>
+        <v>3923</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>3923</v>
+        <v>3922</v>
       </c>
       <c r="D5" s="63" t="s">
-        <v>3961</v>
+        <v>3960</v>
       </c>
       <c r="E5" s="63" t="s">
-        <v>3960</v>
+        <v>3959</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="G5" s="63" t="s">
-        <v>3995</v>
+        <v>3994</v>
       </c>
       <c r="I5" s="59"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
-        <v>4090</v>
+        <v>4089</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>4094</v>
+        <v>4093</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>4093</v>
+        <v>4092</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>4097</v>
+        <v>4096</v>
       </c>
       <c r="E6" s="65" t="s">
-        <v>4096</v>
+        <v>4095</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>4101</v>
+        <v>4100</v>
       </c>
       <c r="G6" s="65" t="s">
-        <v>4100</v>
+        <v>4099</v>
       </c>
       <c r="I6" s="59"/>
     </row>
@@ -46339,22 +46375,22 @@
         <v>3862</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>3926</v>
+        <v>3925</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>3925</v>
+        <v>3924</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>3963</v>
+        <v>3962</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>3962</v>
+        <v>3961</v>
       </c>
       <c r="F8" s="63" t="s">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="G8" s="63" t="s">
-        <v>3997</v>
+        <v>3996</v>
       </c>
       <c r="I8" s="59"/>
     </row>
@@ -46363,22 +46399,22 @@
         <v>3844</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>3928</v>
+        <v>3927</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>3927</v>
+        <v>3926</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>3965</v>
+        <v>3964</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>3964</v>
+        <v>3963</v>
       </c>
       <c r="F9" s="63" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="G9" s="63" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="I9" s="59"/>
     </row>
@@ -46387,22 +46423,22 @@
         <v>3845</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>3930</v>
+        <v>3929</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>3929</v>
+        <v>3928</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>3967</v>
+        <v>3966</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>3966</v>
+        <v>3965</v>
       </c>
       <c r="F10" s="63" t="s">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="G10" s="63" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="I10" s="59"/>
     </row>
@@ -46411,22 +46447,22 @@
         <v>3846</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>3932</v>
+        <v>3931</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>3931</v>
+        <v>3930</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>3969</v>
+        <v>3968</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>3968</v>
+        <v>3967</v>
       </c>
       <c r="F11" s="63" t="s">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="G11" s="63" t="s">
-        <v>4003</v>
+        <v>4002</v>
       </c>
       <c r="I11" s="59"/>
     </row>
@@ -46447,22 +46483,22 @@
         <v>3847</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>3934</v>
+        <v>3933</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>3933</v>
+        <v>3932</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>3971</v>
+        <v>3970</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>3970</v>
+        <v>3969</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>4006</v>
+        <v>4005</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="I13" s="59"/>
     </row>
@@ -46471,22 +46507,22 @@
         <v>3848</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>3936</v>
+        <v>3935</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>3935</v>
+        <v>3934</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>3973</v>
+        <v>3972</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>3972</v>
+        <v>3971</v>
       </c>
       <c r="F14" s="63" t="s">
-        <v>4008</v>
+        <v>4007</v>
       </c>
       <c r="G14" s="63" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="I14" s="59"/>
     </row>
@@ -46495,22 +46531,22 @@
         <v>3849</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>3938</v>
+        <v>3937</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>3937</v>
+        <v>3936</v>
       </c>
       <c r="D15" s="63" t="s">
+        <v>4042</v>
+      </c>
+      <c r="E15" s="63" t="s">
         <v>4043</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="F15" s="63" t="s">
+        <v>4008</v>
+      </c>
+      <c r="G15" s="63" t="s">
         <v>4044</v>
-      </c>
-      <c r="F15" s="63" t="s">
-        <v>4009</v>
-      </c>
-      <c r="G15" s="63" t="s">
-        <v>4045</v>
       </c>
       <c r="I15" s="59"/>
     </row>
@@ -46519,22 +46555,22 @@
         <v>3850</v>
       </c>
       <c r="B16" s="63" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C16" s="63" t="s">
         <v>4046</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="D16" s="63" t="s">
         <v>4047</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="E16" s="63" t="s">
         <v>4048</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="F16" s="63" t="s">
         <v>4049</v>
       </c>
-      <c r="F16" s="63" t="s">
+      <c r="G16" s="63" t="s">
         <v>4050</v>
-      </c>
-      <c r="G16" s="63" t="s">
-        <v>4051</v>
       </c>
       <c r="I16" s="59"/>
     </row>
@@ -46543,22 +46579,22 @@
         <v>3851</v>
       </c>
       <c r="B17" s="63" t="s">
+        <v>4051</v>
+      </c>
+      <c r="C17" s="63" t="s">
         <v>4052</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="D17" s="63" t="s">
         <v>4053</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="E17" s="63" t="s">
         <v>4054</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="F17" s="63" t="s">
         <v>4055</v>
       </c>
-      <c r="F17" s="63" t="s">
+      <c r="G17" s="63" t="s">
         <v>4056</v>
-      </c>
-      <c r="G17" s="63" t="s">
-        <v>4057</v>
       </c>
       <c r="I17" s="59"/>
     </row>
@@ -46567,22 +46603,22 @@
         <v>3853</v>
       </c>
       <c r="B18" s="63" t="s">
+        <v>4057</v>
+      </c>
+      <c r="C18" s="63" t="s">
         <v>4058</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="D18" s="63" t="s">
         <v>4059</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="E18" s="63" t="s">
         <v>4060</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="F18" s="63" t="s">
         <v>4061</v>
       </c>
-      <c r="F18" s="63" t="s">
+      <c r="G18" s="63" t="s">
         <v>4062</v>
-      </c>
-      <c r="G18" s="63" t="s">
-        <v>4063</v>
       </c>
       <c r="I18" s="59"/>
     </row>
@@ -46600,121 +46636,121 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="52" t="s">
-        <v>3918</v>
+        <v>3917</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>3939</v>
+        <v>3938</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>4041</v>
+        <v>4040</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>3974</v>
+        <v>3973</v>
       </c>
       <c r="E20" s="63" t="s">
+        <v>4063</v>
+      </c>
+      <c r="F20" s="63" t="s">
+        <v>4009</v>
+      </c>
+      <c r="G20" s="63" t="s">
         <v>4064</v>
-      </c>
-      <c r="F20" s="63" t="s">
-        <v>4010</v>
-      </c>
-      <c r="G20" s="63" t="s">
-        <v>4065</v>
       </c>
       <c r="I20" s="59"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="52" t="s">
-        <v>3919</v>
+        <v>3918</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>3941</v>
+        <v>3940</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>3940</v>
+        <v>3939</v>
       </c>
       <c r="D21" s="63" t="s">
-        <v>3976</v>
+        <v>3975</v>
       </c>
       <c r="E21" s="63" t="s">
-        <v>3975</v>
+        <v>3974</v>
       </c>
       <c r="F21" s="63" t="s">
-        <v>4012</v>
+        <v>4011</v>
       </c>
       <c r="G21" s="63" t="s">
-        <v>4011</v>
+        <v>4010</v>
       </c>
       <c r="I21" s="59"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="52" t="s">
-        <v>3920</v>
+        <v>3919</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>3943</v>
+        <v>3942</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>3942</v>
+        <v>3941</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>3978</v>
+        <v>3977</v>
       </c>
       <c r="E22" s="63" t="s">
-        <v>3977</v>
+        <v>3976</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>4014</v>
+        <v>4013</v>
       </c>
       <c r="G22" s="63" t="s">
-        <v>4013</v>
+        <v>4012</v>
       </c>
       <c r="I22" s="59"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="52" t="s">
-        <v>3921</v>
+        <v>3920</v>
       </c>
       <c r="B23" s="63" t="s">
+        <v>4065</v>
+      </c>
+      <c r="C23" s="63" t="s">
         <v>4066</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="D23" s="63" t="s">
         <v>4067</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="E23" s="63" t="s">
         <v>4068</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="F23" s="63" t="s">
         <v>4069</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="G23" s="63" t="s">
         <v>4070</v>
-      </c>
-      <c r="G23" s="63" t="s">
-        <v>4071</v>
       </c>
       <c r="I23" s="59"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="52" t="s">
-        <v>3922</v>
+        <v>3921</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>3945</v>
+        <v>3944</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>3944</v>
+        <v>3943</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>3980</v>
+        <v>3979</v>
       </c>
       <c r="E24" s="63" t="s">
-        <v>3979</v>
+        <v>3978</v>
       </c>
       <c r="F24" s="63" t="s">
-        <v>4016</v>
+        <v>4015</v>
       </c>
       <c r="G24" s="63" t="s">
-        <v>4015</v>
+        <v>4014</v>
       </c>
       <c r="I24" s="59"/>
     </row>
@@ -46723,22 +46759,22 @@
         <v>3853</v>
       </c>
       <c r="B25" s="63" t="s">
+        <v>4071</v>
+      </c>
+      <c r="C25" s="63" t="s">
         <v>4072</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="D25" s="63" t="s">
         <v>4073</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="E25" s="63" t="s">
+        <v>4041</v>
+      </c>
+      <c r="F25" s="63" t="s">
         <v>4074</v>
       </c>
-      <c r="E25" s="63" t="s">
-        <v>4042</v>
-      </c>
-      <c r="F25" s="63" t="s">
+      <c r="G25" s="63" t="s">
         <v>4075</v>
-      </c>
-      <c r="G25" s="63" t="s">
-        <v>4076</v>
       </c>
       <c r="I25" s="59"/>
     </row>
@@ -46759,22 +46795,22 @@
         <v>3852</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>3947</v>
+        <v>3946</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>3946</v>
+        <v>3945</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="E27" s="63" t="s">
-        <v>3981</v>
+        <v>3980</v>
       </c>
       <c r="F27" s="63" t="s">
-        <v>4018</v>
+        <v>4017</v>
       </c>
       <c r="G27" s="63" t="s">
-        <v>4017</v>
+        <v>4016</v>
       </c>
       <c r="I27" s="59"/>
     </row>
@@ -46783,22 +46819,22 @@
         <v>3854</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>3949</v>
+        <v>3948</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>3948</v>
+        <v>3947</v>
       </c>
       <c r="D28" s="63" t="s">
-        <v>3984</v>
+        <v>3983</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>3983</v>
+        <v>3982</v>
       </c>
       <c r="F28" s="63" t="s">
-        <v>4020</v>
+        <v>4019</v>
       </c>
       <c r="G28" s="63" t="s">
-        <v>4019</v>
+        <v>4018</v>
       </c>
       <c r="I28" s="59"/>
     </row>
@@ -46807,22 +46843,22 @@
         <v>3855</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>3951</v>
+        <v>3950</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>3950</v>
+        <v>3949</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>3986</v>
+        <v>3985</v>
       </c>
       <c r="E29" s="63" t="s">
-        <v>3985</v>
+        <v>3984</v>
       </c>
       <c r="F29" s="63" t="s">
-        <v>4022</v>
+        <v>4021</v>
       </c>
       <c r="G29" s="63" t="s">
-        <v>4021</v>
+        <v>4020</v>
       </c>
       <c r="I29" s="59"/>
     </row>
@@ -46843,22 +46879,22 @@
         <v>3856</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>3953</v>
+        <v>3952</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>3952</v>
+        <v>3951</v>
       </c>
       <c r="D31" s="63" t="s">
-        <v>3988</v>
+        <v>3987</v>
       </c>
       <c r="E31" s="63" t="s">
-        <v>3987</v>
+        <v>3986</v>
       </c>
       <c r="F31" s="63" t="s">
-        <v>4024</v>
+        <v>4023</v>
       </c>
       <c r="G31" s="63" t="s">
-        <v>4023</v>
+        <v>4022</v>
       </c>
       <c r="I31" s="59"/>
     </row>
@@ -46867,22 +46903,22 @@
         <v>3857</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>3955</v>
+        <v>3954</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>3954</v>
+        <v>3953</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="E32" s="63" t="s">
-        <v>3989</v>
+        <v>3988</v>
       </c>
       <c r="F32" s="63" t="s">
-        <v>4026</v>
+        <v>4025</v>
       </c>
       <c r="G32" s="63" t="s">
-        <v>4025</v>
+        <v>4024</v>
       </c>
       <c r="I32" s="59"/>
     </row>
@@ -46891,22 +46927,22 @@
         <v>3858</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>3957</v>
+        <v>3956</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="D33" s="63" t="s">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="E33" s="63" t="s">
-        <v>3991</v>
+        <v>3990</v>
       </c>
       <c r="F33" s="63" t="s">
-        <v>4028</v>
+        <v>4027</v>
       </c>
       <c r="G33" s="63" t="s">
-        <v>4027</v>
+        <v>4026</v>
       </c>
       <c r="I33" s="59"/>
     </row>
@@ -46915,22 +46951,22 @@
         <v>3859</v>
       </c>
       <c r="B34" s="63" t="s">
+        <v>4076</v>
+      </c>
+      <c r="C34" s="63" t="s">
+        <v>3957</v>
+      </c>
+      <c r="D34" s="63" t="s">
         <v>4077</v>
       </c>
-      <c r="C34" s="63" t="s">
-        <v>3958</v>
-      </c>
-      <c r="D34" s="63" t="s">
+      <c r="E34" s="63" t="s">
+        <v>3992</v>
+      </c>
+      <c r="F34" s="63" t="s">
         <v>4078</v>
       </c>
-      <c r="E34" s="63" t="s">
-        <v>3993</v>
-      </c>
-      <c r="F34" s="63" t="s">
-        <v>4079</v>
-      </c>
       <c r="G34" s="63" t="s">
-        <v>4029</v>
+        <v>4028</v>
       </c>
       <c r="I34" s="59"/>
     </row>
@@ -46939,22 +46975,22 @@
         <v>3860</v>
       </c>
       <c r="B35" s="63" t="s">
+        <v>4079</v>
+      </c>
+      <c r="C35" s="63" t="s">
         <v>4080</v>
       </c>
-      <c r="C35" s="63" t="s">
+      <c r="D35" s="63" t="s">
         <v>4081</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="E35" s="63" t="s">
         <v>4082</v>
       </c>
-      <c r="E35" s="63" t="s">
+      <c r="F35" s="63" t="s">
         <v>4083</v>
       </c>
-      <c r="F35" s="63" t="s">
+      <c r="G35" s="63" t="s">
         <v>4084</v>
-      </c>
-      <c r="G35" s="63" t="s">
-        <v>4085</v>
       </c>
       <c r="I35" s="59"/>
     </row>
@@ -46963,24 +46999,24 @@
         <v>3861</v>
       </c>
       <c r="B36" s="63" t="s">
+        <v>4085</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>3958</v>
+      </c>
+      <c r="D36" s="63" t="s">
         <v>4086</v>
       </c>
-      <c r="C36" s="63" t="s">
-        <v>3959</v>
-      </c>
-      <c r="D36" s="63" t="s">
+      <c r="E36" s="63" t="s">
+        <v>3993</v>
+      </c>
+      <c r="F36" s="63" t="s">
         <v>4087</v>
       </c>
-      <c r="E36" s="63" t="s">
-        <v>3994</v>
-      </c>
-      <c r="F36" s="63" t="s">
-        <v>4088</v>
-      </c>
       <c r="G36" s="63" t="s">
-        <v>4030</v>
-      </c>
-      <c r="I36" s="72"/>
+        <v>4029</v>
+      </c>
+      <c r="I36" s="67"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="51" t="s">
@@ -46994,22 +47030,22 @@
         <v>3865</v>
       </c>
       <c r="B38" s="64" t="s">
-        <v>3901</v>
+        <v>3900</v>
       </c>
       <c r="C38" s="64" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>3907</v>
+        <v>3906</v>
       </c>
       <c r="E38" s="65" t="s">
+        <v>4031</v>
+      </c>
+      <c r="F38" s="64" t="s">
+        <v>3916</v>
+      </c>
+      <c r="G38" s="65" t="s">
         <v>4032</v>
-      </c>
-      <c r="F38" s="64" t="s">
-        <v>3917</v>
-      </c>
-      <c r="G38" s="65" t="s">
-        <v>4033</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -47017,22 +47053,22 @@
         <v>3866</v>
       </c>
       <c r="B39" s="64" t="s">
+        <v>3901</v>
+      </c>
+      <c r="C39" s="64" t="s">
         <v>3902</v>
       </c>
-      <c r="C39" s="64" t="s">
-        <v>3903</v>
-      </c>
       <c r="D39" s="64" t="s">
-        <v>3908</v>
+        <v>3907</v>
       </c>
       <c r="E39" s="65" t="s">
-        <v>4031</v>
+        <v>4030</v>
       </c>
       <c r="F39" s="64" t="s">
-        <v>3916</v>
+        <v>3915</v>
       </c>
       <c r="G39" s="65" t="s">
-        <v>4034</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -47040,22 +47076,22 @@
         <v>3867</v>
       </c>
       <c r="B40" s="64" t="s">
+        <v>3903</v>
+      </c>
+      <c r="C40" s="64" t="s">
         <v>3904</v>
       </c>
-      <c r="C40" s="64" t="s">
-        <v>3905</v>
-      </c>
       <c r="D40" s="64" t="s">
-        <v>3910</v>
+        <v>3909</v>
       </c>
       <c r="E40" s="66" t="s">
-        <v>3909</v>
+        <v>3908</v>
       </c>
       <c r="F40" s="64" t="s">
-        <v>3915</v>
+        <v>3914</v>
       </c>
       <c r="G40" s="66" t="s">
-        <v>3914</v>
+        <v>3913</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -47068,42 +47104,42 @@
         <v>3864</v>
       </c>
       <c r="B42" s="57" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="C42" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="D42" s="57" t="s">
-        <v>3906</v>
+        <v>3905</v>
       </c>
       <c r="E42" s="61" t="s">
+        <v>3910</v>
+      </c>
+      <c r="F42" s="57" t="s">
+        <v>3912</v>
+      </c>
+      <c r="G42" s="61" t="s">
         <v>3911</v>
-      </c>
-      <c r="F42" s="57" t="s">
-        <v>3913</v>
-      </c>
-      <c r="G42" s="61" t="s">
-        <v>3912</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="55" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="B43" s="57" t="s">
-        <v>3889</v>
+        <v>3888</v>
       </c>
       <c r="C43" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="D43" s="57" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
       <c r="E43" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="F43" s="57" t="s">
-        <v>3896</v>
+        <v>3895</v>
       </c>
       <c r="G43" s="57" t="s">
         <v>3392</v>
@@ -47111,22 +47147,22 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="55" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="B44" s="57" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="C44" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="D44" s="57" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="E44" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="F44" s="57" t="s">
-        <v>3897</v>
+        <v>3896</v>
       </c>
       <c r="G44" s="57" t="s">
         <v>3392</v>
@@ -47134,22 +47170,22 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="55" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="B45" s="57" t="s">
-        <v>3891</v>
+        <v>3890</v>
       </c>
       <c r="C45" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>3895</v>
+        <v>3894</v>
       </c>
       <c r="E45" s="57" t="s">
         <v>3392</v>
       </c>
       <c r="F45" s="57" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="G45" s="57" t="s">
         <v>3392</v>
@@ -47157,7 +47193,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="56" t="s">
-        <v>3892</v>
+        <v>3891</v>
       </c>
       <c r="B46" s="60"/>
       <c r="C46" s="60"/>
@@ -47168,7 +47204,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="55" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -47191,17 +47227,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="10.265625" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.53125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="13.1328125" style="44" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="32" customWidth="1"/>
+    <col min="3" max="3" width="16.06640625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" style="32" customWidth="1"/>
+    <col min="5" max="5" width="22.1328125" style="44" customWidth="1"/>
     <col min="6" max="6" width="2.86328125" style="32" customWidth="1"/>
     <col min="7" max="7" width="10.265625" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.796875" style="32" bestFit="1" customWidth="1"/>
@@ -47211,21 +47247,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="70" t="s">
         <v>3871</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
       <c r="F1" s="47"/>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="70" t="s">
         <v>3870</v>
       </c>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-    </row>
-    <row r="2" spans="1:10" ht="29.25" x14ac:dyDescent="0.4">
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+    </row>
+    <row r="2" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
       <c r="B2" s="42" t="s">
         <v>3873</v>
       </c>
@@ -47266,22 +47302,56 @@
       <c r="I3" s="43"/>
       <c r="J3" s="43"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A4" s="32" t="s">
         <v>3877</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>4106</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>4111</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>4103</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>4107</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A5" s="44" t="s">
         <v>3878</v>
       </c>
+      <c r="B5" s="32" t="s">
+        <v>4105</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>4112</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>4102</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>4109</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A6" s="44" t="s">
         <v>3869</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="44" t="s">
+        <v>4104</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>4113</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>4101</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>4110</v>
+      </c>
       <c r="H6" s="44"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
@@ -47324,12 +47394,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="32" t="s">
-        <v>3881</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="32" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
     </row>
   </sheetData>
@@ -47359,11 +47429,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -47600,20 +47670,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72" t="s">
         <v>3681</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B2" s="32" t="s">
@@ -47798,34 +47868,34 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71" t="s">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72" t="s">
         <v>3681</v>
       </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71" t="s">
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="N13" s="71" t="s">
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="N13" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="O13" s="71"/>
-      <c r="P13" s="71" t="s">
+      <c r="O13" s="72"/>
+      <c r="P13" s="72" t="s">
         <v>3681</v>
       </c>
-      <c r="Q13" s="71"/>
-      <c r="R13" s="71"/>
-      <c r="S13" s="71" t="s">
+      <c r="Q13" s="72"/>
+      <c r="R13" s="72"/>
+      <c r="S13" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="T13" s="71"/>
-      <c r="U13" s="71"/>
+      <c r="T13" s="72"/>
+      <c r="U13" s="72"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B14" s="32" t="s">
@@ -48181,20 +48251,20 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71" t="s">
+      <c r="B25" s="72"/>
+      <c r="C25" s="72" t="s">
         <v>3681</v>
       </c>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71" t="s">
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B26" s="32" t="s">
@@ -48206,20 +48276,20 @@
       <c r="G26" s="32" t="s">
         <v>3699</v>
       </c>
-      <c r="N26" s="71" t="s">
+      <c r="N26" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="O26" s="71"/>
-      <c r="P26" s="71" t="s">
+      <c r="O26" s="72"/>
+      <c r="P26" s="72" t="s">
         <v>3681</v>
       </c>
-      <c r="Q26" s="71"/>
-      <c r="R26" s="71"/>
-      <c r="S26" s="71" t="s">
+      <c r="Q26" s="72"/>
+      <c r="R26" s="72"/>
+      <c r="S26" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="T26" s="71"/>
-      <c r="U26" s="71"/>
+      <c r="T26" s="72"/>
+      <c r="U26" s="72"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27" s="32" t="s">
@@ -48571,20 +48641,20 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A37" s="71" t="s">
+      <c r="A37" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71" t="s">
+      <c r="B37" s="72"/>
+      <c r="C37" s="72" t="s">
         <v>3681</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71" t="s">
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72" t="s">
         <v>377</v>
       </c>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B38" s="32" t="s">
@@ -48775,10 +48845,10 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A48" s="71" t="s">
+      <c r="A48" s="72" t="s">
         <v>3662</v>
       </c>
-      <c r="B48" s="71"/>
+      <c r="B48" s="72"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B49" s="32" t="s">
@@ -48873,18 +48943,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="C37:E37"/>
@@ -48892,6 +48950,18 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="F25:H25"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="S26:U26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -48899,21 +48969,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000918DFE69D23CA498FE8574F69332F5A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c85c3d5046845ec940253ce92485889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1ec804960e8faf3526f8b911669b534" ns3:_="">
     <xsd:import namespace="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
@@ -49059,10 +49114,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -49084,19 +49164,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DAG for all cause mort
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFA26D2-B19F-485A-BAA1-C2B8C76F769F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7B876-5A3B-48F4-8FB4-997B814C33BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="4822" windowWidth="16875" windowHeight="10523" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="5625" yWindow="3877" windowWidth="16875" windowHeight="10523" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
@@ -47381,8 +47381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
added adjustments for bmi and smoking and other chronic conditions if we choose to use thsoe
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0E7F60-52AA-4E23-B0DC-5A7C92EC5EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1FEF0B-C4A2-45CE-8541-2D62D442DD69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2003" yWindow="3593" windowWidth="16875" windowHeight="10522" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="3825" yWindow="1230" windowWidth="16875" windowHeight="8633" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8460" uniqueCount="4166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8486" uniqueCount="4187">
   <si>
     <t>Variable</t>
   </si>
@@ -12552,13 +12552,76 @@
     <t>0.7338 (0.6847 - 0.7864)</t>
   </si>
   <si>
-    <t>2011 - 2014 waves</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0 (0.0)  </t>
   </si>
   <si>
-    <t>Additionally adjusting for chronic conditions in all cause models</t>
+    <t>1.1794 (1.0893 - 1.2769)</t>
+  </si>
+  <si>
+    <t>1.1507 (1.0758 - 1.2307)</t>
+  </si>
+  <si>
+    <t>plus smoking and BMI</t>
+  </si>
+  <si>
+    <t>1.1154 (1.0354 - 1.2016)</t>
+  </si>
+  <si>
+    <t>1.1596 (1.0645 - 1.2631)</t>
+  </si>
+  <si>
+    <t>1.2304 (1.1639 - 1.3006)</t>
+  </si>
+  <si>
+    <t>1.1854 (1.1157 - 1.2594)</t>
+  </si>
+  <si>
+    <t>(without the chronic conditions in dz specific)</t>
+  </si>
+  <si>
+    <t>Additionally adjusting for chronic conditions in all cause models (2000 - 2014)</t>
+  </si>
+  <si>
+    <t>Additionally adjusting for chronic conditions in all cause models (2000 - 2010)</t>
+  </si>
+  <si>
+    <t>1.2188 (1.1083 - 1.3402)</t>
+  </si>
+  <si>
+    <t>1.1859 (1.0712 - 1.3128)</t>
+  </si>
+  <si>
+    <t>1.2663 (1.1911 - 1.3461)</t>
+  </si>
+  <si>
+    <t>1.2072 (1.1297 - 1.2899)</t>
+  </si>
+  <si>
+    <t>1.1439 (1.0539 - 1.2416)</t>
+  </si>
+  <si>
+    <t>1.1835 (1.0995 - 1.2739)</t>
+  </si>
+  <si>
+    <t>1.2402 (1.0726 - 1.4341)</t>
+  </si>
+  <si>
+    <t>1.1176 (0.9794 - 1.2754)</t>
+  </si>
+  <si>
+    <t>1.2558 (1.1384 - 1.3853)</t>
+  </si>
+  <si>
+    <t>1.1647 (1.0112 - 1.3415)</t>
+  </si>
+  <si>
+    <t>1.2915 (1.0989 - 1.5177)</t>
+  </si>
+  <si>
+    <t>1.2778 (1.1460 - 1.4248)</t>
+  </si>
+  <si>
+    <t>2011 - 2014 Waves</t>
   </si>
 </sst>
 </file>
@@ -12701,7 +12764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12895,6 +12958,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -47269,7 +47340,7 @@
         <v>3904</v>
       </c>
       <c r="E42" s="61" t="s">
-        <v>4164</v>
+        <v>4163</v>
       </c>
       <c r="F42" s="57" t="s">
         <v>3909</v>
@@ -47381,10 +47452,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="68" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -47397,7 +47468,7 @@
     <col min="6" max="6" width="2.86328125" style="32" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="32" customWidth="1"/>
     <col min="8" max="8" width="19.796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.59765625" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.46484375" style="32" customWidth="1"/>
     <col min="10" max="10" width="20.53125" style="32" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.06640625" style="32"/>
   </cols>
@@ -47603,121 +47674,271 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="75" t="s">
         <v>3869</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="76" t="s">
         <v>4145</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="76" t="s">
         <v>4153</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="76" t="s">
         <v>4148</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="75" t="s">
         <v>4150</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43" t="s">
+      <c r="F11" s="76"/>
+      <c r="G11" s="76" t="s">
         <v>4158</v>
       </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43" t="s">
+      <c r="H11" s="76"/>
+      <c r="I11" s="76" t="s">
         <v>4157</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="76" t="s">
         <v>4161</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="75"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13" s="46" t="s">
+        <v>4186</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" s="32" t="s">
+        <v>3876</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>4109</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>4104</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>4100</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>4101</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>4108</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>4107</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>4117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A15" s="44" t="s">
+        <v>3877</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>4110</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>4105</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>4099</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>4102</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>4113</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>4112</v>
+      </c>
+      <c r="J15" s="32" t="s">
+        <v>4118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A16" s="48" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>4111</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>4106</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>4098</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>4103</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43" t="s">
+        <v>4116</v>
+      </c>
+      <c r="H16" s="48"/>
+      <c r="I16" s="43" t="s">
+        <v>4115</v>
+      </c>
+      <c r="J16" s="43" t="s">
+        <v>4119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="32" t="s">
         <v>4114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="32" t="s">
-        <v>3880</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="32" t="s">
-        <v>4163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="32" t="s">
-        <v>4109</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>4104</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>4100</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>4101</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>4108</v>
-      </c>
-      <c r="I19" s="32" t="s">
-        <v>4107</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>4117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B20" s="32" t="s">
-        <v>4110</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>4105</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>4099</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>4102</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>4113</v>
-      </c>
-      <c r="I20" s="32" t="s">
-        <v>4112</v>
-      </c>
-      <c r="J20" s="32" t="s">
-        <v>4118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B21" s="44" t="s">
-        <v>4111</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>4098</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>4103</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>4116</v>
-      </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="32" t="s">
-        <v>4115</v>
-      </c>
-      <c r="J21" s="32" t="s">
-        <v>4119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A25" s="32" t="s">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26" s="73" t="s">
+        <v>4172</v>
+      </c>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73" t="s">
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J27" s="32" t="s">
         <v>4165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J28" s="32" t="s">
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30" s="32" t="s">
+        <v>4166</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>4180</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="32" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>4181</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="48" t="s">
+        <v>4182</v>
+      </c>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A33" s="32" t="s">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J34" s="32" t="s">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J35" s="32" t="s">
+        <v>4179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="J36" s="32" t="s">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A37" s="32" t="s">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A38" s="32" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>4184</v>
+      </c>
+      <c r="J38" s="32" t="s">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E39" s="44" t="s">
+        <v>4183</v>
+      </c>
+      <c r="J39" s="32" t="s">
+        <v>4178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="48" t="s">
+        <v>4185</v>
+      </c>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43" t="s">
+        <v>4177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new prettier dag and filled in table 2
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1FEF0B-C4A2-45CE-8541-2D62D442DD69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB65D6A-4C41-48C6-89EE-72AE15560ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="1230" windowWidth="16875" windowHeight="8633" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="3450" yWindow="2168" windowWidth="16875" windowHeight="11535" firstSheet="2" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1 (2010-2014)" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1 (2000-2014)" sheetId="1" r:id="rId3"/>
     <sheet name="table1" sheetId="6" r:id="rId4"/>
-    <sheet name="table2" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
-    <sheet name="CoxPHResults" sheetId="5" r:id="rId7"/>
+    <sheet name="table2_round" sheetId="8" r:id="rId5"/>
+    <sheet name="table2" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
+    <sheet name="CoxPHResults" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8486" uniqueCount="4187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8645" uniqueCount="4246">
   <si>
     <t>Variable</t>
   </si>
@@ -12622,6 +12623,183 @@
   </si>
   <si>
     <t>2011 - 2014 Waves</t>
+  </si>
+  <si>
+    <t>FULL Model: Adjusted for age, sex, insurance status, edu, income, race, region, smoking status, and BMI</t>
+  </si>
+  <si>
+    <t>(2000 - 2014)</t>
+  </si>
+  <si>
+    <t>1.1004 (0.9641 - 1.2561)</t>
+  </si>
+  <si>
+    <t>1.2437 (1.1273 - 1.3722)</t>
+  </si>
+  <si>
+    <t>1.2427 (1.0737 - 1.4383)</t>
+  </si>
+  <si>
+    <t>FULL (2000 -2010)</t>
+  </si>
+  <si>
+    <t>1.1441 (0.9932 - 1.3181)</t>
+  </si>
+  <si>
+    <t>1.2656 (1.1349 - 1.4113)</t>
+  </si>
+  <si>
+    <t>1.2992 (1.1039 - 1.5289)</t>
+  </si>
+  <si>
+    <t>FULL (2011 - 2014)</t>
+  </si>
+  <si>
+    <t>1.0920 (0.7707 - 1.5470)</t>
+  </si>
+  <si>
+    <t>1.0200 (0.7161 - 1.4527)</t>
+  </si>
+  <si>
+    <t>1.2624 (0.9863 - 1.6156)</t>
+  </si>
+  <si>
+    <t>Additionally adjusting for chronic conditions in all cause models (2010 - 2014)</t>
+  </si>
+  <si>
+    <t>1.1060 (0.7804  - 1.5670)</t>
+  </si>
+  <si>
+    <t>1.0241 (0.7216 - 1.4535)</t>
+  </si>
+  <si>
+    <t>1.2733 (0.9952 - 1.6289)</t>
+  </si>
+  <si>
+    <t>0.9856 (0.8273 - 1.1742)</t>
+  </si>
+  <si>
+    <t>1.0884 (0.9338 - 1.2685)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9965 (0.8121 - 1.2228)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0844 (0.9417 - 1.2488)</t>
+  </si>
+  <si>
+    <t>1.0204 (0.87000 - 1.1968)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9676 (0.7986 - 1.1724)</t>
+  </si>
+  <si>
+    <t>0.766 (0.674 - 0.870)</t>
+  </si>
+  <si>
+    <t>0.618 (0.548 - 0.696)</t>
+  </si>
+  <si>
+    <t>0.728 (0.669 - 0.792)</t>
+  </si>
+  <si>
+    <t>0.809 (0.700 - 0.934)</t>
+  </si>
+  <si>
+    <t>0.659 (0.582 - 0.747)</t>
+  </si>
+  <si>
+    <t>0.758 (0.691 - 0.833)</t>
+  </si>
+  <si>
+    <t>0.779 (0.639 - 0.950)</t>
+  </si>
+  <si>
+    <t>0.768 (0.633 - 0.931)</t>
+  </si>
+  <si>
+    <t>0.802 (0.700 - 0.918)</t>
+  </si>
+  <si>
+    <t>1.227(1.076 - 1.399)</t>
+  </si>
+  <si>
+    <t>1.138 (1.006 - 1.286)</t>
+  </si>
+  <si>
+    <t>1.310 (1.196 - 1.434)</t>
+  </si>
+  <si>
+    <t>1.287 (1.111 - 1.492)</t>
+  </si>
+  <si>
+    <t>1.190 (1.045 - 1.355)</t>
+  </si>
+  <si>
+    <t>1.336 (1.208 - 1.477)</t>
+  </si>
+  <si>
+    <t>1.283 (1.030 - 1.600)</t>
+  </si>
+  <si>
+    <t>1.598 (1.292 - 1.977)</t>
+  </si>
+  <si>
+    <t>1.559 (1.350 - 1.801)</t>
+  </si>
+  <si>
+    <t>0.752 (0.694 - 0.815)</t>
+  </si>
+  <si>
+    <t>0.702 (0.658 - 0.750)</t>
+  </si>
+  <si>
+    <t>0.771 (0.732 - 0.813)</t>
+  </si>
+  <si>
+    <t>0.799 (0.731 - 0.875)</t>
+  </si>
+  <si>
+    <t>0.734 (0.685 - 0.786)</t>
+  </si>
+  <si>
+    <t>0.805 (0.760 - 0.852)</t>
+  </si>
+  <si>
+    <t>0.681 (0.605 - 0.767)</t>
+  </si>
+  <si>
+    <t>0.620 (0.562 - 0.684)</t>
+  </si>
+  <si>
+    <t>0.695 (0.643 - 0.752)</t>
+  </si>
+  <si>
+    <t>1.192 (1.096 - 1.296)</t>
+  </si>
+  <si>
+    <t>1.195 (1.118 - 1.277)</t>
+  </si>
+  <si>
+    <t>1.279 (1.210 - 1.351)</t>
+  </si>
+  <si>
+    <t>1.256 (1.143 - 1.379)</t>
+  </si>
+  <si>
+    <t>1.224 (1.139 - 1.315)</t>
+  </si>
+  <si>
+    <t>1.315 (1.238 - 1.397)</t>
+  </si>
+  <si>
+    <t>1.100 (0.966 - 1.252)</t>
+  </si>
+  <si>
+    <t>1.111 (1.002 - 1.233)</t>
+  </si>
+  <si>
+    <t>1.206 (1.112 - 1.308)</t>
   </si>
 </sst>
 </file>
@@ -12764,7 +12942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12943,6 +13121,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -12958,14 +13150,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13347,41 +13546,41 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="11"/>
       <c r="G1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="11"/>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="68"/>
+      <c r="M1" s="74"/>
       <c r="P1" s="11"/>
-      <c r="Q1" s="68" t="s">
+      <c r="Q1" s="74" t="s">
         <v>508</v>
       </c>
-      <c r="R1" s="68"/>
+      <c r="R1" s="74"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="68" t="s">
+      <c r="V1" s="74" t="s">
         <v>649</v>
       </c>
-      <c r="W1" s="68"/>
+      <c r="W1" s="74"/>
       <c r="Z1" s="11"/>
-      <c r="AA1" s="68" t="s">
+      <c r="AA1" s="74" t="s">
         <v>650</v>
       </c>
-      <c r="AB1" s="68"/>
+      <c r="AB1" s="74"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="68" t="s">
+      <c r="AF1" s="74" t="s">
         <v>659</v>
       </c>
-      <c r="AG1" s="68"/>
+      <c r="AG1" s="74"/>
       <c r="AJ1" s="11"/>
       <c r="AK1" s="29" t="s">
         <v>1045</v>
@@ -23199,47 +23398,47 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="11"/>
       <c r="H1" s="29" t="s">
         <v>507</v>
       </c>
       <c r="K1" s="29"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="68" t="s">
+      <c r="N1" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="68"/>
+      <c r="O1" s="74"/>
       <c r="Q1" s="29"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="68" t="s">
+      <c r="T1" s="74" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="68"/>
+      <c r="U1" s="74"/>
       <c r="W1" s="29"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="68" t="s">
+      <c r="Z1" s="74" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="68"/>
+      <c r="AA1" s="74"/>
       <c r="AC1" s="29"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="68" t="s">
+      <c r="AF1" s="74" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="68"/>
+      <c r="AG1" s="74"/>
       <c r="AI1" s="29"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="68" t="s">
+      <c r="AL1" s="74" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="68"/>
+      <c r="AM1" s="74"/>
       <c r="AO1" s="29"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="29" t="s">
@@ -33830,7 +34029,7 @@
   <dimension ref="A1:BN167"/>
   <sheetViews>
     <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73:G79"/>
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -33905,13 +34104,13 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="11"/>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11" t="s">
         <v>507</v>
@@ -33920,38 +34119,38 @@
       <c r="J1" s="6"/>
       <c r="K1" s="12"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="68" t="s">
+      <c r="N1" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="68"/>
+      <c r="O1" s="74"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="12"/>
       <c r="S1" s="11"/>
-      <c r="T1" s="68" t="s">
+      <c r="T1" s="74" t="s">
         <v>508</v>
       </c>
-      <c r="U1" s="68"/>
+      <c r="U1" s="74"/>
       <c r="V1" s="6"/>
       <c r="W1" s="12"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="68" t="s">
+      <c r="Z1" s="74" t="s">
         <v>649</v>
       </c>
-      <c r="AA1" s="68"/>
+      <c r="AA1" s="74"/>
       <c r="AB1" s="6"/>
       <c r="AC1" s="12"/>
       <c r="AE1" s="11"/>
-      <c r="AF1" s="68" t="s">
+      <c r="AF1" s="74" t="s">
         <v>650</v>
       </c>
-      <c r="AG1" s="68"/>
+      <c r="AG1" s="74"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="12"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="68" t="s">
+      <c r="AL1" s="74" t="s">
         <v>659</v>
       </c>
-      <c r="AM1" s="68"/>
+      <c r="AM1" s="74"/>
       <c r="AO1" s="12"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="12" t="s">
@@ -46440,7 +46639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7B31CA-98BF-453E-B5B4-4EB9FEC3C9BB}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="87" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
@@ -46457,18 +46656,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="75" t="s">
         <v>3662</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75" t="s">
         <v>3875</v>
       </c>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69" t="s">
+      <c r="E1" s="75"/>
+      <c r="F1" s="75" t="s">
         <v>3881</v>
       </c>
-      <c r="G1" s="69"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="57" t="s">
@@ -47451,49 +47650,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
-  <dimension ref="A1:J40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4313555-EC6E-4D2C-90A6-517B882FC83C}">
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" style="32" customWidth="1"/>
-    <col min="3" max="3" width="16.06640625" style="32" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" style="32" customWidth="1"/>
     <col min="4" max="4" width="21.3984375" style="32" customWidth="1"/>
     <col min="5" max="5" width="22.1328125" style="44" customWidth="1"/>
     <col min="6" max="6" width="2.86328125" style="32" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="32" customWidth="1"/>
-    <col min="8" max="8" width="19.796875" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.46484375" style="32" customWidth="1"/>
-    <col min="10" max="10" width="20.53125" style="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.06640625" style="32"/>
+    <col min="7" max="7" width="11.6640625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="20.46484375" style="32" customWidth="1"/>
+    <col min="9" max="9" width="20.53125" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="70" t="s">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="76" t="s">
         <v>3871</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="47"/>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="76" t="s">
         <v>3870</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-    </row>
-    <row r="2" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="B2" s="42" t="s">
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+    </row>
+    <row r="2" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="B2" s="45" t="s">
+        <v>3874</v>
+      </c>
+      <c r="C2" s="73" t="s">
         <v>3873</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>3874</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>3878</v>
@@ -47501,21 +47697,18 @@
       <c r="E2" s="45" t="s">
         <v>3879</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42" t="s">
+      <c r="F2" s="73"/>
+      <c r="G2" s="73" t="s">
         <v>3873</v>
       </c>
       <c r="H2" s="45" t="s">
-        <v>3874</v>
+        <v>3878</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>3878</v>
-      </c>
-      <c r="J2" s="45" t="s">
         <v>3879</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="46" t="s">
         <v>3872</v>
       </c>
@@ -47527,17 +47720,722 @@
       <c r="G3" s="43"/>
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="32" t="s">
         <v>3876</v>
       </c>
+      <c r="B4" s="73" t="s">
+        <v>4129</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>4120</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>4210</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>4219</v>
+      </c>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73" t="s">
+        <v>4132</v>
+      </c>
+      <c r="H4" s="73" t="s">
+        <v>4228</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>4237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A5" s="44" t="s">
+        <v>3877</v>
+      </c>
+      <c r="B5" s="73" t="s">
+        <v>4130</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>4123</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>4211</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>4220</v>
+      </c>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73" t="s">
+        <v>4134</v>
+      </c>
+      <c r="H5" s="73" t="s">
+        <v>4229</v>
+      </c>
+      <c r="I5" s="73" t="s">
+        <v>4238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A6" s="44" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B6" s="73" t="s">
+        <v>4131</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>4125</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>4212</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>4221</v>
+      </c>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73" t="s">
+        <v>4137</v>
+      </c>
+      <c r="H6" s="73" t="s">
+        <v>4230</v>
+      </c>
+      <c r="I6" s="73" t="s">
+        <v>4239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="46" t="s">
+        <v>4146</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="32" t="s">
+        <v>3876</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>4151</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>4141</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>4213</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>4222</v>
+      </c>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73" t="s">
+        <v>4154</v>
+      </c>
+      <c r="H9" s="73" t="s">
+        <v>4231</v>
+      </c>
+      <c r="I9" s="73" t="s">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A10" s="44" t="s">
+        <v>3877</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>4152</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>4144</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>4214</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>4223</v>
+      </c>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73" t="s">
+        <v>4156</v>
+      </c>
+      <c r="H10" s="73" t="s">
+        <v>4232</v>
+      </c>
+      <c r="I10" s="73" t="s">
+        <v>4241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A11" s="70" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>4153</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>4145</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>4215</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>4224</v>
+      </c>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47" t="s">
+        <v>4158</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>4233</v>
+      </c>
+      <c r="I11" s="47" t="s">
+        <v>4242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="70"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="46" t="s">
+        <v>4186</v>
+      </c>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="32" t="s">
+        <v>3876</v>
+      </c>
+      <c r="B14" s="73" t="s">
+        <v>4104</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>4109</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>4216</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>4225</v>
+      </c>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73" t="s">
+        <v>4108</v>
+      </c>
+      <c r="H14" s="73" t="s">
+        <v>4234</v>
+      </c>
+      <c r="I14" s="73" t="s">
+        <v>4243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A15" s="44" t="s">
+        <v>3877</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>4105</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>4110</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>4217</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>4226</v>
+      </c>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73" t="s">
+        <v>4113</v>
+      </c>
+      <c r="H15" s="73" t="s">
+        <v>4235</v>
+      </c>
+      <c r="I15" s="73" t="s">
+        <v>4244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A16" s="48" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>4106</v>
+      </c>
+      <c r="C16" s="82" t="s">
+        <v>4111</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>4218</v>
+      </c>
+      <c r="E16" s="82" t="s">
+        <v>4227</v>
+      </c>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72" t="s">
+        <v>4116</v>
+      </c>
+      <c r="H16" s="72" t="s">
+        <v>4236</v>
+      </c>
+      <c r="I16" s="72" t="s">
+        <v>4245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="32" t="s">
+        <v>4114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="32" t="s">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="68" t="s">
+        <v>4172</v>
+      </c>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68" t="s">
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I27" s="32" t="s">
+        <v>4165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I28" s="32" t="s">
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="32" t="s">
+        <v>4166</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>4180</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="32" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>4181</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="48" t="s">
+        <v>4182</v>
+      </c>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="32" t="s">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I34" s="32" t="s">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I35" s="32" t="s">
+        <v>4179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I36" s="32" t="s">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="32" t="s">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="32" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>4184</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E39" s="44" t="s">
+        <v>4183</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>4178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="48" t="s">
+        <v>4185</v>
+      </c>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43" t="s">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="32" t="s">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I42" s="40" t="s">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I43" s="40" t="s">
+        <v>4208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I44" s="40" t="s">
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="32" t="s">
+        <v>4166</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>4201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="32" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>4202</v>
+      </c>
+      <c r="I46" s="40" t="s">
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E47" s="40" t="s">
+        <v>4203</v>
+      </c>
+      <c r="I47" s="40" t="s">
+        <v>4204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="43"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="81" t="s">
+        <v>4205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" s="32" t="s">
+        <v>4187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A50" s="32" t="s">
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E55" s="40" t="s">
+        <v>4191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E56" s="40" t="s">
+        <v>4189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E57" s="40" t="s">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A58" s="68" t="s">
+        <v>4192</v>
+      </c>
+      <c r="B58" s="68"/>
+      <c r="C58" s="68"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="68"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
+      <c r="E59" s="40"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A60" s="71"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="I60" s="71"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A61" s="71"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="80"/>
+      <c r="F61" s="71"/>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A62" s="71"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="80" t="s">
+        <v>4195</v>
+      </c>
+      <c r="F62" s="71"/>
+      <c r="G62" s="71"/>
+      <c r="H62" s="71"/>
+      <c r="I62" s="71"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E63" s="40" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E64" s="40" t="s">
+        <v>4194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E65" s="40"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A66" s="68" t="s">
+        <v>4196</v>
+      </c>
+      <c r="B66" s="68"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="68"/>
+      <c r="I66" s="68"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D67" s="71"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
+      <c r="I67" s="71"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E68" s="40"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D69" s="71"/>
+      <c r="E69" s="70"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D70" s="71"/>
+      <c r="E70" s="70"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E71" s="40" t="s">
+        <v>4197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E72" s="40" t="s">
+        <v>4198</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E73" s="40" t="s">
+        <v>4199</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
+  <dimension ref="A1:I73"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="83" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" style="32" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" style="32" customWidth="1"/>
+    <col min="5" max="5" width="22.1328125" style="44" customWidth="1"/>
+    <col min="6" max="6" width="2.86328125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="20.46484375" style="32" customWidth="1"/>
+    <col min="9" max="9" width="20.53125" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="76" t="s">
+        <v>3871</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="76" t="s">
+        <v>3870</v>
+      </c>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+    </row>
+    <row r="2" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="B2" s="45" t="s">
+        <v>3874</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>3873</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>3878</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>3879</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42" t="s">
+        <v>3873</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>3878</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>3879</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="46" t="s">
+        <v>3872</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="32" t="s">
+        <v>3876</v>
+      </c>
       <c r="B4" s="32" t="s">
+        <v>4129</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>4120</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>4129</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>4121</v>
@@ -47548,22 +48446,22 @@
       <c r="G4" s="32" t="s">
         <v>4132</v>
       </c>
+      <c r="H4" s="32" t="s">
+        <v>4133</v>
+      </c>
       <c r="I4" s="32" t="s">
-        <v>4133</v>
-      </c>
-      <c r="J4" s="32" t="s">
         <v>4138</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A5" s="44" t="s">
         <v>3877</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>4130</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>4123</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>4130</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>4122</v>
@@ -47574,22 +48472,22 @@
       <c r="G5" s="32" t="s">
         <v>4134</v>
       </c>
+      <c r="H5" s="32" t="s">
+        <v>4135</v>
+      </c>
       <c r="I5" s="32" t="s">
-        <v>4135</v>
-      </c>
-      <c r="J5" s="32" t="s">
         <v>4139</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A6" s="44" t="s">
         <v>3869</v>
       </c>
       <c r="B6" s="32" t="s">
+        <v>4131</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>4125</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>4131</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>4124</v>
@@ -47600,14 +48498,14 @@
       <c r="G6" s="32" t="s">
         <v>4137</v>
       </c>
+      <c r="H6" s="32" t="s">
+        <v>4136</v>
+      </c>
       <c r="I6" s="32" t="s">
-        <v>4136</v>
-      </c>
-      <c r="J6" s="32" t="s">
         <v>4140</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="46" t="s">
         <v>4146</v>
       </c>
@@ -47619,17 +48517,16 @@
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="32" t="s">
         <v>3876</v>
       </c>
       <c r="B9" s="32" t="s">
+        <v>4151</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>4141</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>4151</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>4142</v>
@@ -47640,22 +48537,22 @@
       <c r="G9" s="32" t="s">
         <v>4154</v>
       </c>
+      <c r="H9" s="32" t="s">
+        <v>4155</v>
+      </c>
       <c r="I9" s="32" t="s">
-        <v>4155</v>
-      </c>
-      <c r="J9" s="32" t="s">
         <v>4159</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A10" s="44" t="s">
         <v>3877</v>
       </c>
       <c r="B10" s="32" t="s">
+        <v>4152</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>4144</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>4152</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>4143</v>
@@ -47666,54 +48563,52 @@
       <c r="G10" s="32" t="s">
         <v>4156</v>
       </c>
+      <c r="H10" s="32" t="s">
+        <v>4162</v>
+      </c>
       <c r="I10" s="32" t="s">
-        <v>4162</v>
-      </c>
-      <c r="J10" s="32" t="s">
         <v>4160</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A11" s="75" t="s">
+    <row r="11" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A11" s="70" t="s">
         <v>3869</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="71" t="s">
+        <v>4153</v>
+      </c>
+      <c r="C11" s="71" t="s">
         <v>4145</v>
       </c>
-      <c r="C11" s="76" t="s">
-        <v>4153</v>
-      </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="71" t="s">
         <v>4148</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="70" t="s">
         <v>4150</v>
       </c>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76" t="s">
+      <c r="F11" s="71"/>
+      <c r="G11" s="71" t="s">
         <v>4158</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76" t="s">
+      <c r="H11" s="71" t="s">
         <v>4157</v>
       </c>
-      <c r="J11" s="76" t="s">
+      <c r="I11" s="71" t="s">
         <v>4161</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="75"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="70"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="46" t="s">
         <v>4186</v>
       </c>
@@ -47725,17 +48620,16 @@
       <c r="G13" s="43"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="32" t="s">
         <v>3876</v>
       </c>
       <c r="B14" s="32" t="s">
+        <v>4104</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>4109</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>4104</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>4100</v>
@@ -47746,22 +48640,22 @@
       <c r="G14" s="32" t="s">
         <v>4108</v>
       </c>
+      <c r="H14" s="32" t="s">
+        <v>4107</v>
+      </c>
       <c r="I14" s="32" t="s">
-        <v>4107</v>
-      </c>
-      <c r="J14" s="32" t="s">
         <v>4117</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A15" s="44" t="s">
         <v>3877</v>
       </c>
       <c r="B15" s="32" t="s">
+        <v>4105</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>4110</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>4105</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>4099</v>
@@ -47772,22 +48666,22 @@
       <c r="G15" s="32" t="s">
         <v>4113</v>
       </c>
+      <c r="H15" s="32" t="s">
+        <v>4112</v>
+      </c>
       <c r="I15" s="32" t="s">
-        <v>4112</v>
-      </c>
-      <c r="J15" s="32" t="s">
         <v>4118</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A16" s="48" t="s">
         <v>3869</v>
       </c>
       <c r="B16" s="48" t="s">
+        <v>4106</v>
+      </c>
+      <c r="C16" s="48" t="s">
         <v>4111</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>4106</v>
       </c>
       <c r="D16" s="43" t="s">
         <v>4098</v>
@@ -47799,73 +48693,71 @@
       <c r="G16" s="43" t="s">
         <v>4116</v>
       </c>
-      <c r="H16" s="48"/>
+      <c r="H16" s="43" t="s">
+        <v>4115</v>
+      </c>
       <c r="I16" s="43" t="s">
-        <v>4115</v>
-      </c>
-      <c r="J16" s="43" t="s">
         <v>4119</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="32" t="s">
         <v>4114</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="32" t="s">
         <v>3880</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A26" s="73" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="68" t="s">
         <v>4172</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73" t="s">
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68" t="s">
         <v>4164</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J27" s="32" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I27" s="32" t="s">
         <v>4165</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J28" s="32" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I28" s="32" t="s">
         <v>4169</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
         <v>4166</v>
       </c>
       <c r="E30" s="44" t="s">
         <v>4180</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="I30" s="32" t="s">
         <v>4168</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="32" t="s">
         <v>4171</v>
       </c>
       <c r="E31" s="44" t="s">
         <v>4181</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="I31" s="32" t="s">
         <v>4167</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="43"/>
       <c r="B32" s="43"/>
       <c r="C32" s="43"/>
@@ -47876,56 +48768,55 @@
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43" t="s">
+      <c r="I32" s="43" t="s">
         <v>4170</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="32" t="s">
         <v>4173</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J34" s="32" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I34" s="32" t="s">
         <v>4174</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J35" s="32" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I35" s="32" t="s">
         <v>4179</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J36" s="32" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I36" s="32" t="s">
         <v>4176</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="32" t="s">
         <v>4166</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="32" t="s">
         <v>4171</v>
       </c>
       <c r="E38" s="44" t="s">
         <v>4184</v>
       </c>
-      <c r="J38" s="32" t="s">
+      <c r="I38" s="32" t="s">
         <v>4175</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="E39" s="44" t="s">
         <v>4183</v>
       </c>
-      <c r="J39" s="32" t="s">
+      <c r="I39" s="32" t="s">
         <v>4178</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="43"/>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
@@ -47936,22 +48827,224 @@
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43" t="s">
+      <c r="I40" s="43" t="s">
         <v>4177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="32" t="s">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I42" s="40" t="s">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I43" s="40" t="s">
+        <v>4208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I44" s="40" t="s">
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="32" t="s">
+        <v>4166</v>
+      </c>
+      <c r="E45" s="40" t="s">
+        <v>4201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="32" t="s">
+        <v>4171</v>
+      </c>
+      <c r="E46" s="40" t="s">
+        <v>4202</v>
+      </c>
+      <c r="I46" s="40" t="s">
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E47" s="40" t="s">
+        <v>4203</v>
+      </c>
+      <c r="I47" s="40" t="s">
+        <v>4204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="43"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="81" t="s">
+        <v>4205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" s="32" t="s">
+        <v>4187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A50" s="32" t="s">
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E55" s="40" t="s">
+        <v>4191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E56" s="40" t="s">
+        <v>4189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E57" s="40" t="s">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A58" s="68" t="s">
+        <v>4192</v>
+      </c>
+      <c r="B58" s="68"/>
+      <c r="C58" s="68"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="68"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A59" s="71"/>
+      <c r="B59" s="71"/>
+      <c r="C59" s="71"/>
+      <c r="E59" s="40"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A60" s="71"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="I60" s="71"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A61" s="71"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="80"/>
+      <c r="F61" s="71"/>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A62" s="71"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="80" t="s">
+        <v>4195</v>
+      </c>
+      <c r="F62" s="71"/>
+      <c r="G62" s="71"/>
+      <c r="H62" s="71"/>
+      <c r="I62" s="71"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E63" s="40" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E64" s="40" t="s">
+        <v>4194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E65" s="40"/>
+      <c r="F65" s="71"/>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="71"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A66" s="68" t="s">
+        <v>4196</v>
+      </c>
+      <c r="B66" s="68"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="68"/>
+      <c r="I66" s="68"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D67" s="71"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
+      <c r="I67" s="71"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E68" s="40"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D69" s="71"/>
+      <c r="E69" s="70"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D70" s="71"/>
+      <c r="E70" s="70"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E71" s="40" t="s">
+        <v>4197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E72" s="40" t="s">
+        <v>4198</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E73" s="40" t="s">
+        <v>4199</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95AEECA-C32B-4507-9F23-8CF5B613F9C9}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -47968,11 +49061,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -48182,11 +49275,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DCAAE1-23D0-4F7F-BF1E-04FFE018A78C}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="96" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="96" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
@@ -48209,20 +49302,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78" t="s">
         <v>3681</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72" t="s">
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B2" s="32" t="s">
@@ -48407,34 +49500,34 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72" t="s">
+      <c r="B13" s="78"/>
+      <c r="C13" s="78" t="s">
         <v>3681</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72" t="s">
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="N13" s="72" t="s">
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="N13" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72" t="s">
+      <c r="O13" s="78"/>
+      <c r="P13" s="78" t="s">
         <v>3681</v>
       </c>
-      <c r="Q13" s="72"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="72" t="s">
+      <c r="Q13" s="78"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="T13" s="72"/>
-      <c r="U13" s="72"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B14" s="32" t="s">
@@ -48790,20 +49883,20 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72" t="s">
+      <c r="B25" s="78"/>
+      <c r="C25" s="78" t="s">
         <v>3681</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72" t="s">
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B26" s="32" t="s">
@@ -48815,20 +49908,20 @@
       <c r="G26" s="32" t="s">
         <v>3699</v>
       </c>
-      <c r="N26" s="72" t="s">
+      <c r="N26" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="O26" s="72"/>
-      <c r="P26" s="72" t="s">
+      <c r="O26" s="78"/>
+      <c r="P26" s="78" t="s">
         <v>3681</v>
       </c>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="72" t="s">
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="T26" s="72"/>
-      <c r="U26" s="72"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="78"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A27" s="32" t="s">
@@ -49180,20 +50273,20 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A37" s="72" t="s">
+      <c r="A37" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72" t="s">
+      <c r="B37" s="78"/>
+      <c r="C37" s="78" t="s">
         <v>3681</v>
       </c>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72" t="s">
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78" t="s">
         <v>377</v>
       </c>
-      <c r="G37" s="72"/>
-      <c r="H37" s="72"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.4">
       <c r="B38" s="32" t="s">
@@ -49384,10 +50477,10 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A48" s="72" t="s">
+      <c r="A48" s="78" t="s">
         <v>3662</v>
       </c>
-      <c r="B48" s="72"/>
+      <c r="B48" s="78"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B49" s="32" t="s">

</xml_diff>

<commit_message>
added more robust checks
</commit_message>
<xml_diff>
--- a/output/NHIS_Variables.xlsx
+++ b/output/NHIS_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\Fall_2019\Capstone\nhis2019\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="114_{A2407726-991A-4713-924A-63313A66922E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C00972D3-5DA1-43A1-9932-61C23D2C1D30}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="114_{A2407726-991A-4713-924A-63313A66922E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FCACA24B-BA48-42AE-A821-A63BA5056080}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" firstSheet="1" activeTab="4" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
+    <workbookView xWindow="1747" yWindow="1357" windowWidth="18211" windowHeight="12893" firstSheet="1" activeTab="6" xr2:uid="{EA08A29F-E728-4C0B-869C-5685DA05B4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude NoDz (2010-2014)" sheetId="4" r:id="rId1"/>
@@ -18,9 +18,11 @@
     <sheet name="Sheet1 (2000-2014)" sheetId="1" r:id="rId3"/>
     <sheet name="table1" sheetId="6" r:id="rId4"/>
     <sheet name="NEWtable2" sheetId="9" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId6"/>
-    <sheet name="OLDtable2_round" sheetId="8" r:id="rId7"/>
-    <sheet name="OLDtable2" sheetId="7" r:id="rId8"/>
+    <sheet name="Supp1" sheetId="11" r:id="rId6"/>
+    <sheet name="Supp2" sheetId="12" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId8"/>
+    <sheet name="OLDtable2_round" sheetId="8" r:id="rId9"/>
+    <sheet name="OLDtable2" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8571" uniqueCount="4289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8639" uniqueCount="4319">
   <si>
     <t>Variable</t>
   </si>
@@ -12967,6 +12969,96 @@
   </si>
   <si>
     <t xml:space="preserve"> and chronic conditions (All models: cancer; CVD models: diabetes; Diabetes models: CVD). Abbreviations: CRN, cost-related nonadherence; CVD, cardiovascular disease; IQR, interquartile range. </t>
+  </si>
+  <si>
+    <t>8737 (23.5)</t>
+  </si>
+  <si>
+    <t>1.182 (1.091 - 1.280)</t>
+  </si>
+  <si>
+    <t>15979 (27.6)</t>
+  </si>
+  <si>
+    <t>1.133 (1.066 - 1.205)</t>
+  </si>
+  <si>
+    <t>28340 (19.4)</t>
+  </si>
+  <si>
+    <t>1.232 (1.172 - 1.296)</t>
+  </si>
+  <si>
+    <t>2882 (8.37)</t>
+  </si>
+  <si>
+    <t>1.180 (1.045 - 1.331)</t>
+  </si>
+  <si>
+    <t>4692 (8.93)</t>
+  </si>
+  <si>
+    <t>1.080 (0.968 - 1.206)</t>
+  </si>
+  <si>
+    <t>10028 (7.30)</t>
+  </si>
+  <si>
+    <t>1.265 (1.162 - 1.378)</t>
+  </si>
+  <si>
+    <t>0.602 (0.542 - 0.668)</t>
+  </si>
+  <si>
+    <t>0.750 (0.669 - 0.840)</t>
+  </si>
+  <si>
+    <t>0.748 (0.686 - 0.815)</t>
+  </si>
+  <si>
+    <t>0.646 (0.600 - 0.694)</t>
+  </si>
+  <si>
+    <t>0.705 (0.667 - 0.746)</t>
+  </si>
+  <si>
+    <t>Delete Overly Influential</t>
+  </si>
+  <si>
+    <t>Splines</t>
+  </si>
+  <si>
+    <t>Died: N(%)</t>
+  </si>
+  <si>
+    <t>Model 2: HR (95% CI)</t>
+  </si>
+  <si>
+    <t>Disease-Specific Mortality</t>
+  </si>
+  <si>
+    <t>1. Hazard Ratio adjusted for age, sex, insurance status, education, race, income, and chronic conditions (All models: cancer; CVD models: diabetes; Diabetes models: CVD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.Hazard Ratio adjusted for age, sex, insurance status, education, race, and income category. Abbreviations: CRN, cost-related nonadherence; CVD, cardiovascular disease; IQR, interquartile range. </t>
+  </si>
+  <si>
+    <t>1.300 (1.183 - 1.421)</t>
+  </si>
+  <si>
+    <t>1.228 (1.076 - 1.402)</t>
+  </si>
+  <si>
+    <t>1.119 (0.989 - 1.267)</t>
+  </si>
+  <si>
+    <t>1.158 (1.063 - 1.261)</t>
+  </si>
+  <si>
+    <t>1.147 (1.072 - 1.228)</t>
+  </si>
+  <si>
+    <t>1.229 (1.162 - 1.300)</t>
   </si>
 </sst>
 </file>
@@ -13120,7 +13212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -13387,6 +13479,9 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -13394,6 +13489,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -13777,41 +13875,41 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
       <c r="F1" s="6"/>
       <c r="G1" s="24" t="s">
         <v>504</v>
       </c>
       <c r="K1" s="6"/>
-      <c r="L1" s="96" t="s">
+      <c r="L1" s="97" t="s">
         <v>374</v>
       </c>
-      <c r="M1" s="96"/>
+      <c r="M1" s="97"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="96" t="s">
+      <c r="Q1" s="97" t="s">
         <v>505</v>
       </c>
-      <c r="R1" s="96"/>
+      <c r="R1" s="97"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="96" t="s">
+      <c r="V1" s="97" t="s">
         <v>646</v>
       </c>
-      <c r="W1" s="96"/>
+      <c r="W1" s="97"/>
       <c r="Z1" s="6"/>
-      <c r="AA1" s="96" t="s">
+      <c r="AA1" s="97" t="s">
         <v>647</v>
       </c>
-      <c r="AB1" s="96"/>
+      <c r="AB1" s="97"/>
       <c r="AE1" s="6"/>
-      <c r="AF1" s="96" t="s">
+      <c r="AF1" s="97" t="s">
         <v>656</v>
       </c>
-      <c r="AG1" s="96"/>
+      <c r="AG1" s="97"/>
       <c r="AJ1" s="6"/>
       <c r="AK1" s="24" t="s">
         <v>1042</v>
@@ -23543,6 +23641,1101 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AA1:AB1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
+  <dimension ref="A1:I134"/>
+  <sheetViews>
+    <sheetView topLeftCell="A65" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="22.1328125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="2.86328125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="20.46484375" style="27" customWidth="1"/>
+    <col min="9" max="9" width="20.53125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="99" t="s">
+        <v>3689</v>
+      </c>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="99" t="s">
+        <v>3688</v>
+      </c>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+    </row>
+    <row r="2" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="B2" s="38" t="s">
+        <v>3692</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>3691</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>3696</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>3697</v>
+      </c>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35" t="s">
+        <v>3691</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>3696</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>3697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="39" t="s">
+        <v>3690</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="27" t="s">
+        <v>3694</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>3947</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>3938</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>3939</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>3944</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>3950</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>3951</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A5" s="37" t="s">
+        <v>3695</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>3948</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>3941</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>3940</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>3945</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>3952</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>3953</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A6" s="37" t="s">
+        <v>3687</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>3949</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>3943</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>3942</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>3946</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>3955</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>3954</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="39" t="s">
+        <v>3964</v>
+      </c>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="27" t="s">
+        <v>3694</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>3969</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>3959</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>3960</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>3965</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>3972</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>3973</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A10" s="37" t="s">
+        <v>3695</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>3970</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>3961</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>3967</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>3974</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>3980</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A11" s="63" t="s">
+        <v>3687</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>3971</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>3966</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>3968</v>
+      </c>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64" t="s">
+        <v>3976</v>
+      </c>
+      <c r="H11" s="64" t="s">
+        <v>3975</v>
+      </c>
+      <c r="I11" s="64" t="s">
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="63"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="39" t="s">
+        <v>4004</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="27" t="s">
+        <v>3694</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>3922</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>3927</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>3918</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>3919</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>3926</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>3925</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>3935</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A15" s="37" t="s">
+        <v>3695</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>3923</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>3928</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>3917</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>3920</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>3931</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>3930</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="A16" s="41" t="s">
+        <v>3687</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>3924</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>3929</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>3916</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>3921</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36" t="s">
+        <v>3934</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>3933</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="27" t="s">
+        <v>3932</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="27" t="s">
+        <v>3698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="61" t="s">
+        <v>3990</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I27" s="27" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I28" s="27" t="s">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="27" t="s">
+        <v>3984</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>3998</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="27" t="s">
+        <v>3989</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>3999</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="41" t="s">
+        <v>4000</v>
+      </c>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36" t="s">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="27" t="s">
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I34" s="27" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I35" s="27" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I36" s="27" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="27" t="s">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="27" t="s">
+        <v>3989</v>
+      </c>
+      <c r="E38" s="37" t="s">
+        <v>4002</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>3993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E39" s="37" t="s">
+        <v>4001</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="41" t="s">
+        <v>4003</v>
+      </c>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36" t="s">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="27" t="s">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I42" s="34" t="s">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I43" s="34" t="s">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I44" s="34" t="s">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="27" t="s">
+        <v>3984</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="27" t="s">
+        <v>3989</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>4020</v>
+      </c>
+      <c r="I46" s="34" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E47" s="34" t="s">
+        <v>4021</v>
+      </c>
+      <c r="I47" s="34" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="71" t="s">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" s="27" t="s">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A50" s="27" t="s">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E55" s="34" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E56" s="34" t="s">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E57" s="34" t="s">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A58" s="61" t="s">
+        <v>4010</v>
+      </c>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="61"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A59" s="64"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="64"/>
+      <c r="E59" s="34"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A60" s="64"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="64"/>
+      <c r="H60" s="64"/>
+      <c r="I60" s="64"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A61" s="64"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="64"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="64"/>
+      <c r="I61" s="64"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A62" s="64"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="64"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="70" t="s">
+        <v>4013</v>
+      </c>
+      <c r="F62" s="64"/>
+      <c r="G62" s="64"/>
+      <c r="H62" s="64"/>
+      <c r="I62" s="64"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E63" s="34" t="s">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E64" s="34" t="s">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E65" s="34"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="64"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A66" s="61" t="s">
+        <v>4014</v>
+      </c>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="61"/>
+      <c r="G66" s="61"/>
+      <c r="H66" s="61"/>
+      <c r="I66" s="61"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D67" s="64"/>
+      <c r="E67" s="70"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
+      <c r="I67" s="64"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E68" s="34"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D69" s="64"/>
+      <c r="E69" s="63"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D70" s="64"/>
+      <c r="E70" s="63"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E71" s="34" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E72" s="34" t="s">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E73" s="34" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C83" s="68"/>
+      <c r="E83" s="77"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C84" s="68"/>
+      <c r="E84" s="77"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C85" s="68"/>
+      <c r="E85" s="77"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C86" s="68"/>
+      <c r="E86" s="77"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A87" s="61" t="s">
+        <v>3990</v>
+      </c>
+      <c r="B87" s="61"/>
+      <c r="C87" s="85"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="79"/>
+      <c r="F87" s="61"/>
+      <c r="G87" s="61"/>
+      <c r="H87" s="61"/>
+      <c r="I87" s="61" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C88" s="68"/>
+      <c r="E88" s="77"/>
+      <c r="I88" s="27" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C89" s="68"/>
+      <c r="E89" s="77"/>
+      <c r="I89" s="27" t="s">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C90" s="68"/>
+      <c r="E90" s="77"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A91" s="27" t="s">
+        <v>3984</v>
+      </c>
+      <c r="C91" s="68"/>
+      <c r="E91" s="77" t="s">
+        <v>3998</v>
+      </c>
+      <c r="I91" s="27" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A92" s="27" t="s">
+        <v>3989</v>
+      </c>
+      <c r="C92" s="68"/>
+      <c r="E92" s="77" t="s">
+        <v>3999</v>
+      </c>
+      <c r="I92" s="27" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A93" s="36"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="67"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="75" t="s">
+        <v>4000</v>
+      </c>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36" t="s">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A94" s="27" t="s">
+        <v>3991</v>
+      </c>
+      <c r="C94" s="68"/>
+      <c r="E94" s="77"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C95" s="68"/>
+      <c r="E95" s="77"/>
+      <c r="I95" s="27" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C96" s="68"/>
+      <c r="E96" s="77"/>
+      <c r="I96" s="27" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C97" s="68"/>
+      <c r="E97" s="77"/>
+      <c r="I97" s="27" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A98" s="27" t="s">
+        <v>3984</v>
+      </c>
+      <c r="C98" s="68"/>
+      <c r="E98" s="77"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A99" s="27" t="s">
+        <v>3989</v>
+      </c>
+      <c r="C99" s="68"/>
+      <c r="E99" s="77" t="s">
+        <v>4002</v>
+      </c>
+      <c r="I99" s="27" t="s">
+        <v>3993</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C100" s="68"/>
+      <c r="E100" s="77" t="s">
+        <v>4001</v>
+      </c>
+      <c r="I100" s="27" t="s">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A101" s="36"/>
+      <c r="B101" s="36"/>
+      <c r="C101" s="67"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="75" t="s">
+        <v>4003</v>
+      </c>
+      <c r="F101" s="36"/>
+      <c r="G101" s="36"/>
+      <c r="H101" s="36"/>
+      <c r="I101" s="36" t="s">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A102" s="27" t="s">
+        <v>4018</v>
+      </c>
+      <c r="C102" s="68"/>
+      <c r="E102" s="77"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C103" s="68"/>
+      <c r="E103" s="77"/>
+      <c r="I103" s="34" t="s">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C104" s="68"/>
+      <c r="E104" s="77"/>
+      <c r="I104" s="34" t="s">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C105" s="68"/>
+      <c r="E105" s="77"/>
+      <c r="I105" s="34" t="s">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A106" s="27" t="s">
+        <v>3984</v>
+      </c>
+      <c r="C106" s="68"/>
+      <c r="E106" s="76" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A107" s="27" t="s">
+        <v>3989</v>
+      </c>
+      <c r="C107" s="68"/>
+      <c r="E107" s="76" t="s">
+        <v>4020</v>
+      </c>
+      <c r="I107" s="34" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C108" s="68"/>
+      <c r="E108" s="76" t="s">
+        <v>4021</v>
+      </c>
+      <c r="I108" s="34" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A109" s="36"/>
+      <c r="B109" s="36"/>
+      <c r="C109" s="67"/>
+      <c r="D109" s="36"/>
+      <c r="E109" s="75"/>
+      <c r="F109" s="36"/>
+      <c r="G109" s="36"/>
+      <c r="H109" s="36"/>
+      <c r="I109" s="71" t="s">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A110" s="27" t="s">
+        <v>4005</v>
+      </c>
+      <c r="C110" s="68"/>
+      <c r="E110" s="77"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A111" s="27" t="s">
+        <v>4006</v>
+      </c>
+      <c r="C111" s="68"/>
+      <c r="E111" s="77"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C112" s="68"/>
+      <c r="E112" s="77"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C113" s="68"/>
+      <c r="E113" s="77"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C114" s="68"/>
+      <c r="E114" s="77"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C115" s="68"/>
+      <c r="E115" s="77"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C116" s="68"/>
+      <c r="E116" s="76" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C117" s="68"/>
+      <c r="E117" s="76" t="s">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C118" s="68"/>
+      <c r="E118" s="76" t="s">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A119" s="61" t="s">
+        <v>4010</v>
+      </c>
+      <c r="B119" s="61"/>
+      <c r="C119" s="85"/>
+      <c r="D119" s="61"/>
+      <c r="E119" s="80"/>
+      <c r="F119" s="61"/>
+      <c r="G119" s="61"/>
+      <c r="H119" s="61"/>
+      <c r="I119" s="61"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A120" s="64"/>
+      <c r="B120" s="64"/>
+      <c r="C120" s="40"/>
+      <c r="E120" s="76"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A121" s="64"/>
+      <c r="B121" s="64"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="64"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="64"/>
+      <c r="G121" s="64"/>
+      <c r="H121" s="64"/>
+      <c r="I121" s="64"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A122" s="64"/>
+      <c r="B122" s="64"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="64"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="64"/>
+      <c r="G122" s="64"/>
+      <c r="H122" s="64"/>
+      <c r="I122" s="64"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A123" s="64"/>
+      <c r="B123" s="64"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="64"/>
+      <c r="E123" s="10" t="s">
+        <v>4013</v>
+      </c>
+      <c r="F123" s="64"/>
+      <c r="G123" s="64"/>
+      <c r="H123" s="64"/>
+      <c r="I123" s="64"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C124" s="68"/>
+      <c r="E124" s="76" t="s">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C125" s="68"/>
+      <c r="E125" s="76" t="s">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C126" s="68"/>
+      <c r="E126" s="76"/>
+      <c r="F126" s="64"/>
+      <c r="G126" s="64"/>
+      <c r="H126" s="64"/>
+      <c r="I126" s="64"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A127" s="61" t="s">
+        <v>4014</v>
+      </c>
+      <c r="B127" s="61"/>
+      <c r="C127" s="85"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="80"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="61"/>
+      <c r="H127" s="61"/>
+      <c r="I127" s="61"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C128" s="68"/>
+      <c r="D128" s="64"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="64"/>
+      <c r="G128" s="64"/>
+      <c r="H128" s="64"/>
+      <c r="I128" s="64"/>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C129" s="68"/>
+      <c r="E129" s="76"/>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C130" s="68"/>
+      <c r="D130" s="64"/>
+      <c r="E130" s="78"/>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C131" s="68"/>
+      <c r="D131" s="64"/>
+      <c r="E131" s="78"/>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C132" s="68"/>
+      <c r="E132" s="76" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C133" s="68"/>
+      <c r="E133" s="76" t="s">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C134" s="68"/>
+      <c r="E134" s="76" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23629,47 +24822,47 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
       <c r="G1" s="6"/>
       <c r="H1" s="24" t="s">
         <v>504</v>
       </c>
       <c r="K1" s="24"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="96" t="s">
+      <c r="N1" s="97" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="96"/>
+      <c r="O1" s="97"/>
       <c r="Q1" s="24"/>
       <c r="S1" s="6"/>
-      <c r="T1" s="96" t="s">
+      <c r="T1" s="97" t="s">
         <v>505</v>
       </c>
-      <c r="U1" s="96"/>
+      <c r="U1" s="97"/>
       <c r="W1" s="24"/>
       <c r="Y1" s="6"/>
-      <c r="Z1" s="96" t="s">
+      <c r="Z1" s="97" t="s">
         <v>646</v>
       </c>
-      <c r="AA1" s="96"/>
+      <c r="AA1" s="97"/>
       <c r="AC1" s="24"/>
       <c r="AE1" s="6"/>
-      <c r="AF1" s="96" t="s">
+      <c r="AF1" s="97" t="s">
         <v>647</v>
       </c>
-      <c r="AG1" s="96"/>
+      <c r="AG1" s="97"/>
       <c r="AI1" s="24"/>
       <c r="AK1" s="6"/>
-      <c r="AL1" s="96" t="s">
+      <c r="AL1" s="97" t="s">
         <v>656</v>
       </c>
-      <c r="AM1" s="96"/>
+      <c r="AM1" s="97"/>
       <c r="AO1" s="24"/>
       <c r="AQ1" s="6"/>
       <c r="AR1" s="24" t="s">
@@ -34335,13 +35528,13 @@
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6" t="s">
         <v>504</v>
@@ -34350,38 +35543,38 @@
       <c r="J1" s="1"/>
       <c r="K1" s="7"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="96" t="s">
+      <c r="N1" s="97" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="96"/>
+      <c r="O1" s="97"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="7"/>
       <c r="S1" s="6"/>
-      <c r="T1" s="96" t="s">
+      <c r="T1" s="97" t="s">
         <v>505</v>
       </c>
-      <c r="U1" s="96"/>
+      <c r="U1" s="97"/>
       <c r="V1" s="1"/>
       <c r="W1" s="7"/>
       <c r="Y1" s="6"/>
-      <c r="Z1" s="96" t="s">
+      <c r="Z1" s="97" t="s">
         <v>646</v>
       </c>
-      <c r="AA1" s="96"/>
+      <c r="AA1" s="97"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="7"/>
       <c r="AE1" s="6"/>
-      <c r="AF1" s="96" t="s">
+      <c r="AF1" s="97" t="s">
         <v>647</v>
       </c>
-      <c r="AG1" s="96"/>
+      <c r="AG1" s="97"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="7"/>
       <c r="AK1" s="6"/>
-      <c r="AL1" s="96" t="s">
+      <c r="AL1" s="97" t="s">
         <v>656</v>
       </c>
-      <c r="AM1" s="96"/>
+      <c r="AM1" s="97"/>
       <c r="AO1" s="7"/>
       <c r="AQ1" s="6"/>
       <c r="AR1" s="7" t="s">
@@ -46887,18 +48080,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="98" t="s">
         <v>3659</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97" t="s">
+      <c r="C1" s="98"/>
+      <c r="D1" s="98" t="s">
         <v>3693</v>
       </c>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97" t="s">
+      <c r="E1" s="98"/>
+      <c r="F1" s="98" t="s">
         <v>3699</v>
       </c>
-      <c r="G1" s="97"/>
+      <c r="G1" s="98"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="50" t="s">
@@ -47884,8 +49077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3BD714-F6F6-44CE-A098-1B3ADD4DBD70}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -47903,16 +49096,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="99" t="s">
         <v>3688</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="G1" s="98" t="s">
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="G1" s="99" t="s">
         <v>3689</v>
       </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
       <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="41.65" x14ac:dyDescent="0.4">
@@ -48268,6 +49461,500 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C18634A-E06E-456E-BD15-4C4D876CFD4D}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="68" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" style="27" customWidth="1"/>
+    <col min="5" max="5" width="22.1328125" style="77" customWidth="1"/>
+    <col min="6" max="6" width="4.3984375" style="27" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" style="27" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.53125" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" s="27" t="s">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="99" t="s">
+        <v>3688</v>
+      </c>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="G2" s="99" t="s">
+        <v>3689</v>
+      </c>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="40"/>
+    </row>
+    <row r="3" spans="1:11" ht="41.65" x14ac:dyDescent="0.4">
+      <c r="B3" s="38" t="s">
+        <v>3692</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>3691</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>3696</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>4064</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>3691</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>3696</v>
+      </c>
+      <c r="I3" s="74" t="s">
+        <v>3697</v>
+      </c>
+      <c r="J3" s="68"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" s="39" t="s">
+        <v>3690</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="36"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" s="27" t="s">
+        <v>3694</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>3947</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>4289</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>4303</v>
+      </c>
+      <c r="E5" s="87" t="s">
+        <v>4290</v>
+      </c>
+      <c r="G5" s="68" t="s">
+        <v>4295</v>
+      </c>
+      <c r="H5" s="86" t="s">
+        <v>4302</v>
+      </c>
+      <c r="I5" s="87" t="s">
+        <v>4296</v>
+      </c>
+      <c r="J5" s="68"/>
+    </row>
+    <row r="6" spans="1:11" ht="29.25" x14ac:dyDescent="0.4">
+      <c r="A6" s="37" t="s">
+        <v>4082</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>3948</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>4291</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>4304</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>4292</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>4297</v>
+      </c>
+      <c r="H6" s="86" t="s">
+        <v>4301</v>
+      </c>
+      <c r="I6" s="81" t="s">
+        <v>4298</v>
+      </c>
+      <c r="J6" s="68"/>
+    </row>
+    <row r="7" spans="1:11" ht="43.15" x14ac:dyDescent="0.4">
+      <c r="A7" s="41" t="s">
+        <v>4083</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>3949</v>
+      </c>
+      <c r="C7" s="96" t="s">
+        <v>4293</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>4305</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>4294</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="96" t="s">
+        <v>4299</v>
+      </c>
+      <c r="H7" s="89" t="s">
+        <v>4054</v>
+      </c>
+      <c r="I7" s="90" t="s">
+        <v>4300</v>
+      </c>
+      <c r="J7" s="68"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="68"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" s="27" t="s">
+        <v>4287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" s="27" t="s">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="27" t="s">
+        <v>4084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K16" s="40"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.4">
+      <c r="K22" s="68"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE94E2D2-4740-4855-9F88-2CC5CEC95955}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.73046875" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" customWidth="1"/>
+    <col min="5" max="5" width="4.06640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>4307</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="100" t="s">
+        <v>3688</v>
+      </c>
+      <c r="D2" s="100"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="100" t="s">
+        <v>4310</v>
+      </c>
+      <c r="G2" s="100"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+    </row>
+    <row r="3" spans="1:11" ht="42" x14ac:dyDescent="0.45">
+      <c r="A3" s="27"/>
+      <c r="B3" s="38" t="s">
+        <v>3692</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>4308</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>4309</v>
+      </c>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73" t="s">
+        <v>4308</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>4309</v>
+      </c>
+      <c r="H3" s="83"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="39" t="s">
+        <v>3690</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="27" t="s">
+        <v>3694</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>3947</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>3950</v>
+      </c>
+      <c r="D5" s="87" t="s">
+        <v>4316</v>
+      </c>
+      <c r="E5" s="87"/>
+      <c r="F5" s="68" t="s">
+        <v>3938</v>
+      </c>
+      <c r="G5" s="86" t="s">
+        <v>4314</v>
+      </c>
+      <c r="H5" s="87"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="37" t="s">
+        <v>4082</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>3948</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>3952</v>
+      </c>
+      <c r="D6" s="87" t="s">
+        <v>4317</v>
+      </c>
+      <c r="E6" s="87"/>
+      <c r="F6" s="68" t="s">
+        <v>3941</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>4315</v>
+      </c>
+      <c r="H6" s="81"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="37" t="s">
+        <v>4083</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>3949</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>3955</v>
+      </c>
+      <c r="D7" s="87" t="s">
+        <v>4318</v>
+      </c>
+      <c r="E7" s="87"/>
+      <c r="F7" s="68" t="s">
+        <v>3943</v>
+      </c>
+      <c r="G7" s="86" t="s">
+        <v>4313</v>
+      </c>
+      <c r="H7" s="87"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="74"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="27" t="s">
+        <v>4311</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="27" t="s">
+        <v>4312</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="27" t="s">
+        <v>4084</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D17" s="91"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D19" s="91"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED4C5A6-F533-4C13-ACF9-63B92CA7B247}">
   <dimension ref="A1:AP42"/>
   <sheetViews>
@@ -48958,7 +50645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4313555-EC6E-4D2C-90A6-517B882FC83C}">
   <dimension ref="A1:I73"/>
   <sheetViews>
@@ -48981,17 +50668,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="99" t="s">
         <v>3689</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
       <c r="F1" s="40"/>
-      <c r="G1" s="98" t="s">
+      <c r="G1" s="99" t="s">
         <v>3688</v>
       </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
     </row>
     <row r="2" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
       <c r="B2" s="38" t="s">
@@ -49664,1117 +51351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA8162D-D5C4-4A4B-A8F4-00F9FF4DAA22}">
-  <dimension ref="A1:I134"/>
-  <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" style="27" customWidth="1"/>
-    <col min="5" max="5" width="22.1328125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="2.86328125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="27" customWidth="1"/>
-    <col min="8" max="8" width="20.46484375" style="27" customWidth="1"/>
-    <col min="9" max="9" width="20.53125" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="27"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="98" t="s">
-        <v>3689</v>
-      </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="98" t="s">
-        <v>3688</v>
-      </c>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-    </row>
-    <row r="2" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="B2" s="38" t="s">
-        <v>3692</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>3691</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>3696</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>3697</v>
-      </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35" t="s">
-        <v>3691</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>3696</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>3697</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="39" t="s">
-        <v>3690</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="27" t="s">
-        <v>3694</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>3947</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>3938</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>3939</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>3944</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>3950</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>3951</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>3956</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A5" s="37" t="s">
-        <v>3695</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>3948</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>3941</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>3940</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>3945</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>3952</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>3953</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>3957</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A6" s="37" t="s">
-        <v>3687</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>3949</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>3943</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>3942</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>3946</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>3955</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>3954</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>3958</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="39" t="s">
-        <v>3964</v>
-      </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="27" t="s">
-        <v>3694</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>3969</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>3959</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>3960</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>3965</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>3972</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>3973</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>3977</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A10" s="37" t="s">
-        <v>3695</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>3970</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>3962</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>3961</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>3967</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>3974</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>3980</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>3978</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A11" s="63" t="s">
-        <v>3687</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>3971</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>3963</v>
-      </c>
-      <c r="D11" s="64" t="s">
-        <v>3966</v>
-      </c>
-      <c r="E11" s="63" t="s">
-        <v>3968</v>
-      </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64" t="s">
-        <v>3976</v>
-      </c>
-      <c r="H11" s="64" t="s">
-        <v>3975</v>
-      </c>
-      <c r="I11" s="64" t="s">
-        <v>3979</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="39" t="s">
-        <v>4004</v>
-      </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="27" t="s">
-        <v>3694</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>3922</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>3927</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>3918</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>3919</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>3926</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>3925</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A15" s="37" t="s">
-        <v>3695</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>3923</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>3928</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>3917</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>3920</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>3931</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>3930</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>3936</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="41.65" x14ac:dyDescent="0.4">
-      <c r="A16" s="41" t="s">
-        <v>3687</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>3924</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>3929</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>3916</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>3921</v>
-      </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36" t="s">
-        <v>3934</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>3933</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>3937</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="27" t="s">
-        <v>3932</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="27" t="s">
-        <v>3698</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" s="61" t="s">
-        <v>3990</v>
-      </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61" t="s">
-        <v>3982</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I27" s="27" t="s">
-        <v>3983</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I28" s="27" t="s">
-        <v>3987</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A30" s="27" t="s">
-        <v>3984</v>
-      </c>
-      <c r="E30" s="37" t="s">
-        <v>3998</v>
-      </c>
-      <c r="I30" s="27" t="s">
-        <v>3986</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A31" s="27" t="s">
-        <v>3989</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>3999</v>
-      </c>
-      <c r="I31" s="27" t="s">
-        <v>3985</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="41" t="s">
-        <v>4000</v>
-      </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36" t="s">
-        <v>3988</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="27" t="s">
-        <v>3991</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I34" s="27" t="s">
-        <v>3992</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I35" s="27" t="s">
-        <v>3997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I36" s="27" t="s">
-        <v>3994</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="27" t="s">
-        <v>3984</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="27" t="s">
-        <v>3989</v>
-      </c>
-      <c r="E38" s="37" t="s">
-        <v>4002</v>
-      </c>
-      <c r="I38" s="27" t="s">
-        <v>3993</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E39" s="37" t="s">
-        <v>4001</v>
-      </c>
-      <c r="I39" s="27" t="s">
-        <v>3996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="41" t="s">
-        <v>4003</v>
-      </c>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36" t="s">
-        <v>3995</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="27" t="s">
-        <v>4018</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I42" s="34" t="s">
-        <v>4027</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I43" s="34" t="s">
-        <v>4026</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="I44" s="34" t="s">
-        <v>4025</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="27" t="s">
-        <v>3984</v>
-      </c>
-      <c r="E45" s="34" t="s">
-        <v>4019</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A46" s="27" t="s">
-        <v>3989</v>
-      </c>
-      <c r="E46" s="34" t="s">
-        <v>4020</v>
-      </c>
-      <c r="I46" s="34" t="s">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E47" s="34" t="s">
-        <v>4021</v>
-      </c>
-      <c r="I47" s="34" t="s">
-        <v>4022</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="71" t="s">
-        <v>4023</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A49" s="27" t="s">
-        <v>4005</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A50" s="27" t="s">
-        <v>4006</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E55" s="34" t="s">
-        <v>4009</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E56" s="34" t="s">
-        <v>4007</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E57" s="34" t="s">
-        <v>4008</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A58" s="61" t="s">
-        <v>4010</v>
-      </c>
-      <c r="B58" s="61"/>
-      <c r="C58" s="61"/>
-      <c r="D58" s="61"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="61"/>
-      <c r="H58" s="61"/>
-      <c r="I58" s="61"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A59" s="64"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-      <c r="E59" s="34"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A60" s="64"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="64"/>
-      <c r="H60" s="64"/>
-      <c r="I60" s="64"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A61" s="64"/>
-      <c r="B61" s="64"/>
-      <c r="C61" s="64"/>
-      <c r="D61" s="64"/>
-      <c r="E61" s="70"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="64"/>
-      <c r="H61" s="64"/>
-      <c r="I61" s="64"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A62" s="64"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="64"/>
-      <c r="D62" s="64"/>
-      <c r="E62" s="70" t="s">
-        <v>4013</v>
-      </c>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="64"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E63" s="34" t="s">
-        <v>4011</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E64" s="34" t="s">
-        <v>4012</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E65" s="34"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-      <c r="I65" s="64"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A66" s="61" t="s">
-        <v>4014</v>
-      </c>
-      <c r="B66" s="61"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="61"/>
-      <c r="G66" s="61"/>
-      <c r="H66" s="61"/>
-      <c r="I66" s="61"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D67" s="64"/>
-      <c r="E67" s="70"/>
-      <c r="F67" s="64"/>
-      <c r="G67" s="64"/>
-      <c r="H67" s="64"/>
-      <c r="I67" s="64"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E68" s="34"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D69" s="64"/>
-      <c r="E69" s="63"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D70" s="64"/>
-      <c r="E70" s="63"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E71" s="34" t="s">
-        <v>4015</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E72" s="34" t="s">
-        <v>4016</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E73" s="34" t="s">
-        <v>4017</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C83" s="68"/>
-      <c r="E83" s="77"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C84" s="68"/>
-      <c r="E84" s="77"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C85" s="68"/>
-      <c r="E85" s="77"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C86" s="68"/>
-      <c r="E86" s="77"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A87" s="61" t="s">
-        <v>3990</v>
-      </c>
-      <c r="B87" s="61"/>
-      <c r="C87" s="85"/>
-      <c r="D87" s="61"/>
-      <c r="E87" s="79"/>
-      <c r="F87" s="61"/>
-      <c r="G87" s="61"/>
-      <c r="H87" s="61"/>
-      <c r="I87" s="61" t="s">
-        <v>3982</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C88" s="68"/>
-      <c r="E88" s="77"/>
-      <c r="I88" s="27" t="s">
-        <v>3983</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C89" s="68"/>
-      <c r="E89" s="77"/>
-      <c r="I89" s="27" t="s">
-        <v>3987</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C90" s="68"/>
-      <c r="E90" s="77"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A91" s="27" t="s">
-        <v>3984</v>
-      </c>
-      <c r="C91" s="68"/>
-      <c r="E91" s="77" t="s">
-        <v>3998</v>
-      </c>
-      <c r="I91" s="27" t="s">
-        <v>3986</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A92" s="27" t="s">
-        <v>3989</v>
-      </c>
-      <c r="C92" s="68"/>
-      <c r="E92" s="77" t="s">
-        <v>3999</v>
-      </c>
-      <c r="I92" s="27" t="s">
-        <v>3985</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A93" s="36"/>
-      <c r="B93" s="36"/>
-      <c r="C93" s="67"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="75" t="s">
-        <v>4000</v>
-      </c>
-      <c r="F93" s="36"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="36"/>
-      <c r="I93" s="36" t="s">
-        <v>3988</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A94" s="27" t="s">
-        <v>3991</v>
-      </c>
-      <c r="C94" s="68"/>
-      <c r="E94" s="77"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C95" s="68"/>
-      <c r="E95" s="77"/>
-      <c r="I95" s="27" t="s">
-        <v>3992</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C96" s="68"/>
-      <c r="E96" s="77"/>
-      <c r="I96" s="27" t="s">
-        <v>3997</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C97" s="68"/>
-      <c r="E97" s="77"/>
-      <c r="I97" s="27" t="s">
-        <v>3994</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A98" s="27" t="s">
-        <v>3984</v>
-      </c>
-      <c r="C98" s="68"/>
-      <c r="E98" s="77"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A99" s="27" t="s">
-        <v>3989</v>
-      </c>
-      <c r="C99" s="68"/>
-      <c r="E99" s="77" t="s">
-        <v>4002</v>
-      </c>
-      <c r="I99" s="27" t="s">
-        <v>3993</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C100" s="68"/>
-      <c r="E100" s="77" t="s">
-        <v>4001</v>
-      </c>
-      <c r="I100" s="27" t="s">
-        <v>3996</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A101" s="36"/>
-      <c r="B101" s="36"/>
-      <c r="C101" s="67"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="75" t="s">
-        <v>4003</v>
-      </c>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36" t="s">
-        <v>3995</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A102" s="27" t="s">
-        <v>4018</v>
-      </c>
-      <c r="C102" s="68"/>
-      <c r="E102" s="77"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C103" s="68"/>
-      <c r="E103" s="77"/>
-      <c r="I103" s="34" t="s">
-        <v>4027</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C104" s="68"/>
-      <c r="E104" s="77"/>
-      <c r="I104" s="34" t="s">
-        <v>4026</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C105" s="68"/>
-      <c r="E105" s="77"/>
-      <c r="I105" s="34" t="s">
-        <v>4025</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A106" s="27" t="s">
-        <v>3984</v>
-      </c>
-      <c r="C106" s="68"/>
-      <c r="E106" s="76" t="s">
-        <v>4019</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A107" s="27" t="s">
-        <v>3989</v>
-      </c>
-      <c r="C107" s="68"/>
-      <c r="E107" s="76" t="s">
-        <v>4020</v>
-      </c>
-      <c r="I107" s="34" t="s">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C108" s="68"/>
-      <c r="E108" s="76" t="s">
-        <v>4021</v>
-      </c>
-      <c r="I108" s="34" t="s">
-        <v>4022</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A109" s="36"/>
-      <c r="B109" s="36"/>
-      <c r="C109" s="67"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="75"/>
-      <c r="F109" s="36"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="71" t="s">
-        <v>4023</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A110" s="27" t="s">
-        <v>4005</v>
-      </c>
-      <c r="C110" s="68"/>
-      <c r="E110" s="77"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A111" s="27" t="s">
-        <v>4006</v>
-      </c>
-      <c r="C111" s="68"/>
-      <c r="E111" s="77"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C112" s="68"/>
-      <c r="E112" s="77"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C113" s="68"/>
-      <c r="E113" s="77"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C114" s="68"/>
-      <c r="E114" s="77"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C115" s="68"/>
-      <c r="E115" s="77"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C116" s="68"/>
-      <c r="E116" s="76" t="s">
-        <v>4009</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C117" s="68"/>
-      <c r="E117" s="76" t="s">
-        <v>4007</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C118" s="68"/>
-      <c r="E118" s="76" t="s">
-        <v>4008</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A119" s="61" t="s">
-        <v>4010</v>
-      </c>
-      <c r="B119" s="61"/>
-      <c r="C119" s="85"/>
-      <c r="D119" s="61"/>
-      <c r="E119" s="80"/>
-      <c r="F119" s="61"/>
-      <c r="G119" s="61"/>
-      <c r="H119" s="61"/>
-      <c r="I119" s="61"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A120" s="64"/>
-      <c r="B120" s="64"/>
-      <c r="C120" s="40"/>
-      <c r="E120" s="76"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A121" s="64"/>
-      <c r="B121" s="64"/>
-      <c r="C121" s="40"/>
-      <c r="D121" s="64"/>
-      <c r="E121" s="10"/>
-      <c r="F121" s="64"/>
-      <c r="G121" s="64"/>
-      <c r="H121" s="64"/>
-      <c r="I121" s="64"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A122" s="64"/>
-      <c r="B122" s="64"/>
-      <c r="C122" s="40"/>
-      <c r="D122" s="64"/>
-      <c r="E122" s="10"/>
-      <c r="F122" s="64"/>
-      <c r="G122" s="64"/>
-      <c r="H122" s="64"/>
-      <c r="I122" s="64"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A123" s="64"/>
-      <c r="B123" s="64"/>
-      <c r="C123" s="40"/>
-      <c r="D123" s="64"/>
-      <c r="E123" s="10" t="s">
-        <v>4013</v>
-      </c>
-      <c r="F123" s="64"/>
-      <c r="G123" s="64"/>
-      <c r="H123" s="64"/>
-      <c r="I123" s="64"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C124" s="68"/>
-      <c r="E124" s="76" t="s">
-        <v>4011</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C125" s="68"/>
-      <c r="E125" s="76" t="s">
-        <v>4012</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C126" s="68"/>
-      <c r="E126" s="76"/>
-      <c r="F126" s="64"/>
-      <c r="G126" s="64"/>
-      <c r="H126" s="64"/>
-      <c r="I126" s="64"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A127" s="61" t="s">
-        <v>4014</v>
-      </c>
-      <c r="B127" s="61"/>
-      <c r="C127" s="85"/>
-      <c r="D127" s="61"/>
-      <c r="E127" s="80"/>
-      <c r="F127" s="61"/>
-      <c r="G127" s="61"/>
-      <c r="H127" s="61"/>
-      <c r="I127" s="61"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C128" s="68"/>
-      <c r="D128" s="64"/>
-      <c r="E128" s="10"/>
-      <c r="F128" s="64"/>
-      <c r="G128" s="64"/>
-      <c r="H128" s="64"/>
-      <c r="I128" s="64"/>
-    </row>
-    <row r="129" spans="3:5" x14ac:dyDescent="0.4">
-      <c r="C129" s="68"/>
-      <c r="E129" s="76"/>
-    </row>
-    <row r="130" spans="3:5" x14ac:dyDescent="0.4">
-      <c r="C130" s="68"/>
-      <c r="D130" s="64"/>
-      <c r="E130" s="78"/>
-    </row>
-    <row r="131" spans="3:5" x14ac:dyDescent="0.4">
-      <c r="C131" s="68"/>
-      <c r="D131" s="64"/>
-      <c r="E131" s="78"/>
-    </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.4">
-      <c r="C132" s="68"/>
-      <c r="E132" s="76" t="s">
-        <v>4015</v>
-      </c>
-    </row>
-    <row r="133" spans="3:5" x14ac:dyDescent="0.4">
-      <c r="C133" s="68"/>
-      <c r="E133" s="76" t="s">
-        <v>4016</v>
-      </c>
-    </row>
-    <row r="134" spans="3:5" x14ac:dyDescent="0.4">
-      <c r="C134" s="68"/>
-      <c r="E134" s="76" t="s">
-        <v>4017</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="C1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000918DFE69D23CA498FE8574F69332F5A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c85c3d5046845ec940253ce92485889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1ec804960e8faf3526f8b911669b534" ns3:_="">
     <xsd:import namespace="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
@@ -50920,31 +51497,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8882C1FE-BC45-4FCD-A08C-67DB8BD38111}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35180B2B-1E9F-4F31-82AD-E5A4A56A900A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50960,4 +51528,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77295791-F19B-40DD-BDD7-633F94102999}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8882C1FE-BC45-4FCD-A08C-67DB8BD38111}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="10f9cd9a-7ad2-47ce-9abb-80d6fe5fd300"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>